<commit_message>
Minor correction on the variables dictionnaries (fix upper/lowercase)
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="484">
   <si>
     <t>name</t>
   </si>
@@ -1415,15 +1415,9 @@
     <t>sleept_psc</t>
   </si>
   <si>
-    <t>Decimal</t>
-  </si>
-  <si>
     <t>h/day</t>
   </si>
   <si>
-    <t>sleep (day + night), h/day, preschool age</t>
-  </si>
-  <si>
     <t>sleeptage_psc</t>
   </si>
   <si>
@@ -1433,9 +1427,6 @@
     <t>outdoorp_psc</t>
   </si>
   <si>
-    <t>time spent playing outdoors h/day, preschool age</t>
-  </si>
-  <si>
     <t>outdoorpage_psc</t>
   </si>
   <si>
@@ -1445,15 +1436,9 @@
     <t>tv_psc</t>
   </si>
   <si>
-    <t>time spent watching TV, h/day, preschool age</t>
-  </si>
-  <si>
     <t>screenoth_psc</t>
   </si>
   <si>
-    <t>time spent watching screens (except TV) h/day, preschool age</t>
-  </si>
-  <si>
     <t>screenage_psc</t>
   </si>
   <si>
@@ -1463,13 +1448,25 @@
     <t>patternA_snackscreen_psc</t>
   </si>
   <si>
-    <t>child’s score on the snack screen pattern (relative, derived from PCA loadings), preschool age</t>
-  </si>
-  <si>
     <t>patternB_psc</t>
   </si>
   <si>
-    <t>child’s score on the second multibehavioral pattern (relative, derived from PCA loadings), preschool age</t>
+    <t>Sleep (day + night), h/day, preschool age</t>
+  </si>
+  <si>
+    <t>Time spent playing outdoors h/day, preschool age</t>
+  </si>
+  <si>
+    <t>Time spent watching TV, h/day, preschool age</t>
+  </si>
+  <si>
+    <t>Time spent watching screens (except TV) h/day, preschool age</t>
+  </si>
+  <si>
+    <t>Child’s score on the snack screen pattern (relative, derived from PCA loadings), preschool age</t>
+  </si>
+  <si>
+    <t>Child’s score on the second multibehavioral pattern (relative, derived from PCA loadings), preschool age</t>
   </si>
 </sst>
 </file>
@@ -2069,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG120"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3852,105 +3849,105 @@
         <v>465</v>
       </c>
       <c r="B112" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="C112" s="13" t="s">
-        <v>467</v>
-      </c>
       <c r="D112" s="13" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>466</v>
+        <v>11</v>
       </c>
       <c r="C113" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B114" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C114" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="C114" s="14" t="s">
-        <v>467</v>
-      </c>
       <c r="D114" s="13" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>466</v>
+        <v>11</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B116" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C116" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="C116" s="13" t="s">
-        <v>467</v>
-      </c>
       <c r="D116" s="13" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B117" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="C117" s="13" t="s">
-        <v>467</v>
-      </c>
       <c r="D117" s="13" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>466</v>
+        <v>11</v>
       </c>
       <c r="C118" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D118" s="14" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>466</v>
+        <v>11</v>
       </c>
       <c r="C119" s="13"/>
       <c r="D119" s="14" t="s">
@@ -3959,14 +3956,14 @@
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>466</v>
+        <v>11</v>
       </c>
       <c r="C120" s="13"/>
       <c r="D120" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(boolean): converted text to real boolean
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0987AAF-69E2-FA4C-B363-04986BB79F39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="16152" windowHeight="10236" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16160" windowHeight="10240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2156" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="817">
   <si>
     <t>name</t>
   </si>
@@ -1977,9 +1983,6 @@
   </si>
   <si>
     <t>isMissing</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
   <si>
     <t>Gen R</t>
@@ -2474,7 +2477,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -2549,16 +2552,24 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2600,7 +2611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2632,9 +2643,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2666,6 +2695,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2841,20 +2888,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D313"/>
   <sheetViews>
     <sheetView topLeftCell="A283" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="197.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="197.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -7248,21 +7295,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D224" sqref="D224"/>
+      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D299" sqref="D299"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -7286,11 +7333,11 @@
       <c r="B2" s="2">
         <v>101</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -7300,11 +7347,11 @@
       <c r="B3" s="2">
         <v>102</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>654</v>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
@@ -7314,11 +7361,11 @@
       <c r="B4" s="2">
         <v>103</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>654</v>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
@@ -7328,11 +7375,11 @@
       <c r="B5" s="2">
         <v>104</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>654</v>
+      <c r="C5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -7342,11 +7389,11 @@
       <c r="B6" s="2">
         <v>105</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>654</v>
+      <c r="C6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
@@ -7356,11 +7403,11 @@
       <c r="B7" s="2">
         <v>106</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>654</v>
+      <c r="C7" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -7370,11 +7417,11 @@
       <c r="B8" s="2">
         <v>107</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>654</v>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
@@ -7384,11 +7431,11 @@
       <c r="B9" s="2">
         <v>108</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>654</v>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
@@ -7398,11 +7445,11 @@
       <c r="B10" s="2">
         <v>109</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>654</v>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
@@ -7412,11 +7459,11 @@
       <c r="B11" s="2">
         <v>110</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>654</v>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
@@ -7426,11 +7473,11 @@
       <c r="B12" s="2">
         <v>111</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>654</v>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
@@ -7440,11 +7487,11 @@
       <c r="B13" s="2">
         <v>112</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>654</v>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
@@ -7454,11 +7501,11 @@
       <c r="B14" s="2">
         <v>113</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>654</v>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
@@ -7468,11 +7515,11 @@
       <c r="B15" s="2">
         <v>114</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>654</v>
+      <c r="C15" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
@@ -7482,11 +7529,11 @@
       <c r="B16" s="2">
         <v>115</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>654</v>
+      <c r="C16" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -7496,11 +7543,11 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>654</v>
+      <c r="C17" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -7510,11 +7557,11 @@
       <c r="B18" s="2">
         <v>117</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>654</v>
+      <c r="C18" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
@@ -7524,11 +7571,11 @@
       <c r="B19" s="2">
         <v>118</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>654</v>
+      <c r="C19" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
@@ -7538,11 +7585,11 @@
       <c r="B20" s="2">
         <v>119</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>654</v>
+      <c r="C20" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
@@ -7552,11 +7599,11 @@
       <c r="B21" s="2">
         <v>120</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>654</v>
+      <c r="C21" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
@@ -7566,11 +7613,11 @@
       <c r="B22" s="2">
         <v>121</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>654</v>
+      <c r="C22" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
@@ -7580,11 +7627,11 @@
       <c r="B23" s="2">
         <v>122</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>654</v>
+      <c r="C23" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
@@ -7594,11 +7641,11 @@
       <c r="B24" s="2">
         <v>36</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>654</v>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
@@ -7608,11 +7655,11 @@
       <c r="B25" s="2">
         <v>208</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>654</v>
+      <c r="C25" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -7622,11 +7669,11 @@
       <c r="B26" s="2">
         <v>246</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>654</v>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
@@ -7636,11 +7683,11 @@
       <c r="B27" s="2">
         <v>250</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>654</v>
+      <c r="C27" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
@@ -7650,11 +7697,11 @@
       <c r="B28" s="2">
         <v>276</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>654</v>
+      <c r="C28" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
@@ -7664,11 +7711,11 @@
       <c r="B29" s="2">
         <v>300</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>654</v>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
@@ -7678,11 +7725,11 @@
       <c r="B30" s="2">
         <v>380</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>654</v>
+      <c r="C30" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
@@ -7692,11 +7739,11 @@
       <c r="B31" s="2">
         <v>528</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>654</v>
+      <c r="C31" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1">
@@ -7706,11 +7753,11 @@
       <c r="B32" s="2">
         <v>578</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>654</v>
+      <c r="C32" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
@@ -7720,11 +7767,11 @@
       <c r="B33" s="2">
         <v>724</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>654</v>
+      <c r="C33" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
@@ -7734,11 +7781,11 @@
       <c r="B34" s="2">
         <v>826</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>654</v>
+      <c r="C34" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1">
@@ -7748,11 +7795,11 @@
       <c r="B35" s="2">
         <v>0</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>654</v>
+      <c r="C35" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
@@ -7762,11 +7809,11 @@
       <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>654</v>
+      <c r="C36" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
@@ -7776,11 +7823,11 @@
       <c r="B37" s="2">
         <v>2</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>654</v>
+      <c r="C37" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
@@ -7790,11 +7837,11 @@
       <c r="B38" s="2">
         <v>1</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>654</v>
+      <c r="C38" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1">
@@ -7804,11 +7851,11 @@
       <c r="B39" s="2">
         <v>2</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>654</v>
+      <c r="C39" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1">
@@ -7818,11 +7865,11 @@
       <c r="B40" s="2">
         <v>3</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>654</v>
+      <c r="C40" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
@@ -7832,11 +7879,11 @@
       <c r="B41" s="2">
         <v>1</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>654</v>
+      <c r="C41" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
@@ -7846,11 +7893,11 @@
       <c r="B42" s="2">
         <v>2</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>654</v>
+      <c r="C42" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1">
@@ -7860,11 +7907,11 @@
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>654</v>
+      <c r="C43" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1">
@@ -7874,11 +7921,11 @@
       <c r="B44" s="2">
         <v>1</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>654</v>
+      <c r="C44" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1">
@@ -7888,11 +7935,11 @@
       <c r="B45" s="2">
         <v>2</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>654</v>
+      <c r="C45" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1">
@@ -7902,11 +7949,11 @@
       <c r="B46" s="2">
         <v>3</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>654</v>
+      <c r="C46" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
@@ -7916,11 +7963,11 @@
       <c r="B47" s="2">
         <v>0</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>654</v>
+      <c r="C47" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1">
@@ -7930,11 +7977,11 @@
       <c r="B48" s="2">
         <v>1</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>654</v>
+      <c r="C48" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
@@ -7944,11 +7991,11 @@
       <c r="B49" s="2">
         <v>0</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>654</v>
+      <c r="C49" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
@@ -7958,11 +8005,11 @@
       <c r="B50" s="2">
         <v>1</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>654</v>
+      <c r="C50" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
@@ -7972,11 +8019,11 @@
       <c r="B51" s="2">
         <v>0</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>654</v>
+      <c r="C51" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
@@ -7986,11 +8033,11 @@
       <c r="B52" s="2">
         <v>1</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>654</v>
+      <c r="C52" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
@@ -8000,11 +8047,11 @@
       <c r="B53" s="2">
         <v>0</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>654</v>
+      <c r="C53" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
@@ -8014,11 +8061,11 @@
       <c r="B54" s="2">
         <v>1</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>654</v>
+      <c r="C54" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
@@ -8028,11 +8075,11 @@
       <c r="B55" s="2">
         <v>2</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>654</v>
+      <c r="C55" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
@@ -8042,11 +8089,11 @@
       <c r="B56" s="2">
         <v>3</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>654</v>
+      <c r="C56" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
@@ -8056,11 +8103,11 @@
       <c r="B57" s="2">
         <v>0</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>654</v>
+      <c r="C57" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
@@ -8070,11 +8117,11 @@
       <c r="B58" s="2">
         <v>1</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>654</v>
+      <c r="C58" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
@@ -8084,11 +8131,11 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>654</v>
+      <c r="C59" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
@@ -8098,11 +8145,11 @@
       <c r="B60" s="2">
         <v>2</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>654</v>
+      <c r="C60" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
@@ -8112,11 +8159,11 @@
       <c r="B61" s="2">
         <v>3</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>654</v>
+      <c r="C61" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1">
@@ -8126,8 +8173,8 @@
       <c r="B62" s="2">
         <v>4</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>654</v>
+      <c r="C62" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>380</v>
@@ -8140,11 +8187,11 @@
       <c r="B63" s="2">
         <v>5</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>654</v>
+      <c r="C63" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
@@ -8154,11 +8201,11 @@
       <c r="B64" s="2">
         <v>0</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>654</v>
+      <c r="C64" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1">
@@ -8168,11 +8215,11 @@
       <c r="B65" s="2">
         <v>1</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>654</v>
+      <c r="C65" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1">
@@ -8182,11 +8229,11 @@
       <c r="B66" s="2">
         <v>0</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>654</v>
+      <c r="C66" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1">
@@ -8196,11 +8243,11 @@
       <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>654</v>
+      <c r="C67" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1">
@@ -8210,11 +8257,11 @@
       <c r="B68" s="2">
         <v>0</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>654</v>
+      <c r="C68" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1">
@@ -8224,11 +8271,11 @@
       <c r="B69" s="2">
         <v>1</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>654</v>
+      <c r="C69" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1">
@@ -8238,11 +8285,11 @@
       <c r="B70" s="2">
         <v>0</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>654</v>
+      <c r="C70" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1">
@@ -8252,11 +8299,11 @@
       <c r="B71" s="2">
         <v>1</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>654</v>
+      <c r="C71" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1">
@@ -8266,11 +8313,11 @@
       <c r="B72" s="2">
         <v>0</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>654</v>
+      <c r="C72" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1">
@@ -8280,11 +8327,11 @@
       <c r="B73" s="2">
         <v>1</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>654</v>
+      <c r="C73" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1">
@@ -8294,11 +8341,11 @@
       <c r="B74" s="2">
         <v>0</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>654</v>
+      <c r="C74" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1">
@@ -8308,11 +8355,11 @@
       <c r="B75" s="2">
         <v>1</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>654</v>
+      <c r="C75" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1">
@@ -8322,11 +8369,11 @@
       <c r="B76" s="2">
         <v>0</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>654</v>
+      <c r="C76" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1">
@@ -8336,11 +8383,11 @@
       <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>654</v>
+      <c r="C77" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1">
@@ -8350,11 +8397,11 @@
       <c r="B78" s="2">
         <v>0</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>654</v>
+      <c r="C78" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1">
@@ -8364,11 +8411,11 @@
       <c r="B79" s="2">
         <v>1</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>654</v>
+      <c r="C79" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1">
@@ -8378,11 +8425,11 @@
       <c r="B80" s="2">
         <v>0</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>654</v>
+      <c r="C80" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1">
@@ -8392,11 +8439,11 @@
       <c r="B81" s="2">
         <v>1</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>654</v>
+      <c r="C81" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1">
@@ -8406,11 +8453,11 @@
       <c r="B82" s="2">
         <v>0</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>654</v>
+      <c r="C82" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1">
@@ -8420,11 +8467,11 @@
       <c r="B83" s="2">
         <v>1</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>654</v>
+      <c r="C83" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1">
@@ -8434,11 +8481,11 @@
       <c r="B84" s="2">
         <v>0</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>654</v>
+      <c r="C84" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" customHeight="1">
@@ -8448,11 +8495,11 @@
       <c r="B85" s="2">
         <v>1</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>654</v>
+      <c r="C85" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1">
@@ -8462,11 +8509,11 @@
       <c r="B86" s="2">
         <v>2</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>654</v>
+      <c r="C86" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1">
@@ -8476,11 +8523,11 @@
       <c r="B87" s="2">
         <v>0</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>654</v>
+      <c r="C87" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1">
@@ -8490,11 +8537,11 @@
       <c r="B88" s="2">
         <v>1</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>654</v>
+      <c r="C88" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" customHeight="1">
@@ -8504,11 +8551,11 @@
       <c r="B89" s="2">
         <v>0</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>654</v>
+      <c r="C89" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1">
@@ -8518,11 +8565,11 @@
       <c r="B90" s="2">
         <v>1</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>654</v>
+      <c r="C90" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1">
@@ -8532,11 +8579,11 @@
       <c r="B91" s="2">
         <v>2</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>654</v>
+      <c r="C91" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1">
@@ -8546,11 +8593,11 @@
       <c r="B92" s="2">
         <v>0</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>654</v>
+      <c r="C92" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" customHeight="1">
@@ -8560,11 +8607,11 @@
       <c r="B93" s="2">
         <v>1</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>654</v>
+      <c r="C93" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" customHeight="1">
@@ -8574,11 +8621,11 @@
       <c r="B94" s="2">
         <v>0</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>654</v>
+      <c r="C94" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" customHeight="1">
@@ -8588,11 +8635,11 @@
       <c r="B95" s="2">
         <v>1</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>654</v>
+      <c r="C95" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" customHeight="1">
@@ -8602,11 +8649,11 @@
       <c r="B96" s="2">
         <v>2</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>654</v>
+      <c r="C96" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" customHeight="1">
@@ -8616,11 +8663,11 @@
       <c r="B97" s="2">
         <v>3</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>654</v>
+      <c r="C97" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" customHeight="1">
@@ -8630,11 +8677,11 @@
       <c r="B98" s="2">
         <v>4</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>654</v>
+      <c r="C98" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" customHeight="1">
@@ -8644,11 +8691,11 @@
       <c r="B99" s="2">
         <v>0</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>654</v>
+      <c r="C99" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" customHeight="1">
@@ -8658,11 +8705,11 @@
       <c r="B100" s="2">
         <v>1</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>654</v>
+      <c r="C100" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" customHeight="1">
@@ -8672,11 +8719,11 @@
       <c r="B101" s="2">
         <v>0</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>654</v>
+      <c r="C101" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1">
@@ -8686,11 +8733,11 @@
       <c r="B102" s="2">
         <v>1</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>654</v>
+      <c r="C102" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" customHeight="1">
@@ -8700,11 +8747,11 @@
       <c r="B103" s="2">
         <v>2</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>654</v>
+      <c r="C103" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1">
@@ -8714,11 +8761,11 @@
       <c r="B104" s="2">
         <v>3</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>654</v>
+      <c r="C104" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" customHeight="1">
@@ -8728,11 +8775,11 @@
       <c r="B105" s="2">
         <v>0</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>654</v>
+      <c r="C105" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1">
@@ -8742,11 +8789,11 @@
       <c r="B106" s="2">
         <v>1</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>654</v>
+      <c r="C106" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" customHeight="1">
@@ -8756,11 +8803,11 @@
       <c r="B107" s="2">
         <v>0</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>654</v>
+      <c r="C107" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" customHeight="1">
@@ -8770,11 +8817,11 @@
       <c r="B108" s="2">
         <v>1</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>654</v>
+      <c r="C108" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" customHeight="1">
@@ -8784,11 +8831,11 @@
       <c r="B109" s="2">
         <v>0</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>654</v>
+      <c r="C109" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" customHeight="1">
@@ -8798,11 +8845,11 @@
       <c r="B110" s="2">
         <v>1</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>654</v>
+      <c r="C110" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" customHeight="1">
@@ -8812,11 +8859,11 @@
       <c r="B111" s="2">
         <v>0</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>654</v>
+      <c r="C111" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" customHeight="1">
@@ -8826,11 +8873,11 @@
       <c r="B112" s="2">
         <v>1</v>
       </c>
-      <c r="C112" s="2" t="s">
-        <v>654</v>
+      <c r="C112" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1">
@@ -8840,11 +8887,11 @@
       <c r="B113" s="2">
         <v>2</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>654</v>
+      <c r="C113" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1">
@@ -8854,11 +8901,11 @@
       <c r="B114" s="2">
         <v>3</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>654</v>
+      <c r="C114" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1">
@@ -8868,11 +8915,11 @@
       <c r="B115" s="2">
         <v>4</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>654</v>
+      <c r="C115" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1">
@@ -8882,11 +8929,11 @@
       <c r="B116" s="2">
         <v>1</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>654</v>
+      <c r="C116" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1">
@@ -8896,11 +8943,11 @@
       <c r="B117" s="2">
         <v>2</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>654</v>
+      <c r="C117" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1">
@@ -8910,11 +8957,11 @@
       <c r="B118" s="2">
         <v>0</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>654</v>
+      <c r="C118" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1">
@@ -8924,11 +8971,11 @@
       <c r="B119" s="2">
         <v>1</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>654</v>
+      <c r="C119" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1">
@@ -8938,11 +8985,11 @@
       <c r="B120" s="2">
         <v>0</v>
       </c>
-      <c r="C120" s="2" t="s">
-        <v>654</v>
+      <c r="C120" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1">
@@ -8952,11 +8999,11 @@
       <c r="B121" s="2">
         <v>1</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>654</v>
+      <c r="C121" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1">
@@ -8966,11 +9013,11 @@
       <c r="B122" s="2">
         <v>1</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>654</v>
+      <c r="C122" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1">
@@ -8980,11 +9027,11 @@
       <c r="B123" s="2">
         <v>2</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>654</v>
+      <c r="C123" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1">
@@ -8994,11 +9041,11 @@
       <c r="B124" s="2">
         <v>3</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>654</v>
+      <c r="C124" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1">
@@ -9008,11 +9055,11 @@
       <c r="B125" s="2">
         <v>4</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>654</v>
+      <c r="C125" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1">
@@ -9022,11 +9069,11 @@
       <c r="B126" s="2">
         <v>5</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>654</v>
+      <c r="C126" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1">
@@ -9036,11 +9083,11 @@
       <c r="B127" s="2">
         <v>6</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>654</v>
+      <c r="C127" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1">
@@ -9050,11 +9097,11 @@
       <c r="B128" s="2">
         <v>1</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>654</v>
+      <c r="C128" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1">
@@ -9064,11 +9111,11 @@
       <c r="B129" s="2">
         <v>2</v>
       </c>
-      <c r="C129" s="2" t="s">
-        <v>654</v>
+      <c r="C129" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1">
@@ -9078,11 +9125,11 @@
       <c r="B130" s="2">
         <v>3</v>
       </c>
-      <c r="C130" s="2" t="s">
-        <v>654</v>
+      <c r="C130" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1">
@@ -9092,11 +9139,11 @@
       <c r="B131" s="2">
         <v>4</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>654</v>
+      <c r="C131" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1">
@@ -9106,11 +9153,11 @@
       <c r="B132" s="2">
         <v>5</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>654</v>
+      <c r="C132" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1">
@@ -9120,11 +9167,11 @@
       <c r="B133" s="2">
         <v>0</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>654</v>
+      <c r="C133" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1">
@@ -9134,11 +9181,11 @@
       <c r="B134" s="2">
         <v>1</v>
       </c>
-      <c r="C134" s="2" t="s">
-        <v>654</v>
+      <c r="C134" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1">
@@ -9148,11 +9195,11 @@
       <c r="B135" s="2">
         <v>0</v>
       </c>
-      <c r="C135" s="2" t="s">
-        <v>654</v>
+      <c r="C135" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1">
@@ -9162,11 +9209,11 @@
       <c r="B136" s="2">
         <v>1</v>
       </c>
-      <c r="C136" s="2" t="s">
-        <v>654</v>
+      <c r="C136" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1">
@@ -9176,11 +9223,11 @@
       <c r="B137" s="2">
         <v>2</v>
       </c>
-      <c r="C137" s="2" t="s">
-        <v>654</v>
+      <c r="C137" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1">
@@ -9190,11 +9237,11 @@
       <c r="B138" s="2">
         <v>1</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>654</v>
+      <c r="C138" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1">
@@ -9204,11 +9251,11 @@
       <c r="B139" s="2">
         <v>2</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>654</v>
+      <c r="C139" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1">
@@ -9218,11 +9265,11 @@
       <c r="B140" s="2">
         <v>3</v>
       </c>
-      <c r="C140" s="2" t="s">
-        <v>654</v>
+      <c r="C140" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1">
@@ -9232,11 +9279,11 @@
       <c r="B141" s="2">
         <v>4</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>654</v>
+      <c r="C141" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1">
@@ -9246,11 +9293,11 @@
       <c r="B142" s="2">
         <v>1</v>
       </c>
-      <c r="C142" s="2" t="s">
-        <v>654</v>
+      <c r="C142" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1">
@@ -9260,11 +9307,11 @@
       <c r="B143" s="2">
         <v>2</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>654</v>
+      <c r="C143" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1">
@@ -9274,11 +9321,11 @@
       <c r="B144" s="2">
         <v>3</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>654</v>
+      <c r="C144" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1">
@@ -9288,11 +9335,11 @@
       <c r="B145" s="2">
         <v>1</v>
       </c>
-      <c r="C145" s="2" t="s">
-        <v>654</v>
+      <c r="C145" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1">
@@ -9302,11 +9349,11 @@
       <c r="B146" s="2">
         <v>2</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>654</v>
+      <c r="C146" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1">
@@ -9316,11 +9363,11 @@
       <c r="B147" s="2">
         <v>3</v>
       </c>
-      <c r="C147" s="2" t="s">
-        <v>654</v>
+      <c r="C147" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1">
@@ -9330,11 +9377,11 @@
       <c r="B148" s="2">
         <v>1</v>
       </c>
-      <c r="C148" s="2" t="s">
-        <v>654</v>
+      <c r="C148" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1">
@@ -9344,11 +9391,11 @@
       <c r="B149" s="2">
         <v>2</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>654</v>
+      <c r="C149" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1">
@@ -9358,11 +9405,11 @@
       <c r="B150" s="2">
         <v>3</v>
       </c>
-      <c r="C150" s="2" t="s">
-        <v>654</v>
+      <c r="C150" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1">
@@ -9372,11 +9419,11 @@
       <c r="B151" s="2">
         <v>1</v>
       </c>
-      <c r="C151" s="2" t="s">
-        <v>654</v>
+      <c r="C151" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1">
@@ -9386,11 +9433,11 @@
       <c r="B152" s="2">
         <v>2</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>654</v>
+      <c r="C152" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1">
@@ -9400,11 +9447,11 @@
       <c r="B153" s="2">
         <v>3</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>654</v>
+      <c r="C153" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1">
@@ -9414,11 +9461,11 @@
       <c r="B154" s="2">
         <v>4</v>
       </c>
-      <c r="C154" s="2" t="s">
-        <v>654</v>
+      <c r="C154" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1">
@@ -9428,11 +9475,11 @@
       <c r="B155" s="2">
         <v>0</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>654</v>
+      <c r="C155" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" customHeight="1">
@@ -9442,11 +9489,11 @@
       <c r="B156" s="2">
         <v>1</v>
       </c>
-      <c r="C156" s="2" t="s">
-        <v>654</v>
+      <c r="C156" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15" customHeight="1">
@@ -9456,11 +9503,11 @@
       <c r="B157" s="2">
         <v>1</v>
       </c>
-      <c r="C157" s="2" t="s">
-        <v>654</v>
+      <c r="C157" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15" customHeight="1">
@@ -9470,11 +9517,11 @@
       <c r="B158" s="2">
         <v>2</v>
       </c>
-      <c r="C158" s="2" t="s">
-        <v>654</v>
+      <c r="C158" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1">
@@ -9484,11 +9531,11 @@
       <c r="B159" s="2">
         <v>3</v>
       </c>
-      <c r="C159" s="2" t="s">
-        <v>654</v>
+      <c r="C159" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1">
@@ -9498,11 +9545,11 @@
       <c r="B160" s="2">
         <v>4</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>654</v>
+      <c r="C160" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" customHeight="1">
@@ -9512,11 +9559,11 @@
       <c r="B161" s="2">
         <v>0</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>654</v>
+      <c r="C161" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="15" customHeight="1">
@@ -9526,11 +9573,11 @@
       <c r="B162" s="2">
         <v>1</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>654</v>
+      <c r="C162" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="15" customHeight="1">
@@ -9540,11 +9587,11 @@
       <c r="B163" s="2">
         <v>2</v>
       </c>
-      <c r="C163" s="2" t="s">
-        <v>654</v>
+      <c r="C163" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="15" customHeight="1">
@@ -9554,11 +9601,11 @@
       <c r="B164" s="2">
         <v>1</v>
       </c>
-      <c r="C164" s="2" t="s">
-        <v>654</v>
+      <c r="C164" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15" customHeight="1">
@@ -9568,11 +9615,11 @@
       <c r="B165" s="2">
         <v>2</v>
       </c>
-      <c r="C165" s="2" t="s">
-        <v>654</v>
+      <c r="C165" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15" customHeight="1">
@@ -9582,11 +9629,11 @@
       <c r="B166" s="2">
         <v>3</v>
       </c>
-      <c r="C166" s="2" t="s">
-        <v>654</v>
+      <c r="C166" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15" customHeight="1">
@@ -9596,11 +9643,11 @@
       <c r="B167" s="2">
         <v>4</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>654</v>
+      <c r="C167" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15" customHeight="1">
@@ -9610,11 +9657,11 @@
       <c r="B168" s="2">
         <v>0</v>
       </c>
-      <c r="C168" s="2" t="s">
-        <v>654</v>
+      <c r="C168" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15" customHeight="1">
@@ -9624,11 +9671,11 @@
       <c r="B169" s="2">
         <v>1</v>
       </c>
-      <c r="C169" s="2" t="s">
-        <v>654</v>
+      <c r="C169" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15" customHeight="1">
@@ -9638,11 +9685,11 @@
       <c r="B170" s="2">
         <v>2</v>
       </c>
-      <c r="C170" s="2" t="s">
-        <v>654</v>
+      <c r="C170" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15" customHeight="1">
@@ -9652,11 +9699,11 @@
       <c r="B171" s="2">
         <v>1</v>
       </c>
-      <c r="C171" s="2" t="s">
-        <v>654</v>
+      <c r="C171" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15" customHeight="1">
@@ -9666,11 +9713,11 @@
       <c r="B172" s="2">
         <v>2</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>654</v>
+      <c r="C172" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15" customHeight="1">
@@ -9680,11 +9727,11 @@
       <c r="B173" s="2">
         <v>3</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>654</v>
+      <c r="C173" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15" customHeight="1">
@@ -9694,11 +9741,11 @@
       <c r="B174" s="2">
         <v>4</v>
       </c>
-      <c r="C174" s="2" t="s">
-        <v>654</v>
+      <c r="C174" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15" customHeight="1">
@@ -9708,11 +9755,11 @@
       <c r="B175" s="2">
         <v>1</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>654</v>
+      <c r="C175" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15" customHeight="1">
@@ -9722,11 +9769,11 @@
       <c r="B176" s="2">
         <v>2</v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>654</v>
+      <c r="C176" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15" customHeight="1">
@@ -9736,11 +9783,11 @@
       <c r="B177" s="2">
         <v>3</v>
       </c>
-      <c r="C177" s="2" t="s">
-        <v>654</v>
+      <c r="C177" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15" customHeight="1">
@@ -9750,11 +9797,11 @@
       <c r="B178" s="2">
         <v>4</v>
       </c>
-      <c r="C178" s="2" t="s">
-        <v>654</v>
+      <c r="C178" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15" customHeight="1">
@@ -9764,11 +9811,11 @@
       <c r="B179" s="2">
         <v>0</v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>654</v>
+      <c r="C179" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15" customHeight="1">
@@ -9778,11 +9825,11 @@
       <c r="B180" s="2">
         <v>1</v>
       </c>
-      <c r="C180" s="2" t="s">
-        <v>654</v>
+      <c r="C180" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15" customHeight="1">
@@ -9792,11 +9839,11 @@
       <c r="B181" s="2">
         <v>0</v>
       </c>
-      <c r="C181" s="2" t="s">
-        <v>654</v>
+      <c r="C181" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15" customHeight="1">
@@ -9806,11 +9853,11 @@
       <c r="B182" s="2">
         <v>1</v>
       </c>
-      <c r="C182" s="2" t="s">
-        <v>654</v>
+      <c r="C182" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1">
@@ -9820,11 +9867,11 @@
       <c r="B183" s="2">
         <v>0</v>
       </c>
-      <c r="C183" s="2" t="s">
-        <v>654</v>
+      <c r="C183" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15" customHeight="1">
@@ -9834,11 +9881,11 @@
       <c r="B184" s="2">
         <v>1</v>
       </c>
-      <c r="C184" s="2" t="s">
-        <v>654</v>
+      <c r="C184" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15" customHeight="1">
@@ -9848,11 +9895,11 @@
       <c r="B185" s="2">
         <v>0</v>
       </c>
-      <c r="C185" s="2" t="s">
-        <v>654</v>
+      <c r="C185" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15" customHeight="1">
@@ -9862,11 +9909,11 @@
       <c r="B186" s="2">
         <v>1</v>
       </c>
-      <c r="C186" s="2" t="s">
-        <v>654</v>
+      <c r="C186" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15" customHeight="1">
@@ -9876,11 +9923,11 @@
       <c r="B187" s="2">
         <v>2</v>
       </c>
-      <c r="C187" s="2" t="s">
-        <v>654</v>
+      <c r="C187" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15" customHeight="1">
@@ -9890,11 +9937,11 @@
       <c r="B188" s="2">
         <v>1</v>
       </c>
-      <c r="C188" s="2" t="s">
-        <v>654</v>
+      <c r="C188" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15" customHeight="1">
@@ -9904,11 +9951,11 @@
       <c r="B189" s="2">
         <v>2</v>
       </c>
-      <c r="C189" s="2" t="s">
-        <v>654</v>
+      <c r="C189" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15" customHeight="1">
@@ -9918,11 +9965,11 @@
       <c r="B190" s="2">
         <v>3</v>
       </c>
-      <c r="C190" s="2" t="s">
-        <v>654</v>
+      <c r="C190" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15" customHeight="1">
@@ -9932,11 +9979,11 @@
       <c r="B191" s="2">
         <v>4</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>654</v>
+      <c r="C191" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15" customHeight="1">
@@ -9946,11 +9993,11 @@
       <c r="B192" s="2">
         <v>0</v>
       </c>
-      <c r="C192" s="2" t="s">
-        <v>654</v>
+      <c r="C192" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15" customHeight="1">
@@ -9960,11 +10007,11 @@
       <c r="B193" s="2">
         <v>1</v>
       </c>
-      <c r="C193" s="2" t="s">
-        <v>654</v>
+      <c r="C193" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15" customHeight="1">
@@ -9974,11 +10021,11 @@
       <c r="B194" s="2">
         <v>1</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>654</v>
+      <c r="C194" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15" customHeight="1">
@@ -9988,11 +10035,11 @@
       <c r="B195" s="2">
         <v>2</v>
       </c>
-      <c r="C195" s="2" t="s">
-        <v>654</v>
+      <c r="C195" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15" customHeight="1">
@@ -10002,11 +10049,11 @@
       <c r="B196" s="2">
         <v>1</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>654</v>
+      <c r="C196" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15" customHeight="1">
@@ -10016,11 +10063,11 @@
       <c r="B197" s="2">
         <v>2</v>
       </c>
-      <c r="C197" s="2" t="s">
-        <v>654</v>
+      <c r="C197" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15" customHeight="1">
@@ -10030,11 +10077,11 @@
       <c r="B198" s="2">
         <v>3</v>
       </c>
-      <c r="C198" s="2" t="s">
-        <v>654</v>
+      <c r="C198" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15" customHeight="1">
@@ -10044,11 +10091,11 @@
       <c r="B199" s="2">
         <v>1</v>
       </c>
-      <c r="C199" s="2" t="s">
-        <v>654</v>
+      <c r="C199" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15" customHeight="1">
@@ -10058,11 +10105,11 @@
       <c r="B200" s="2">
         <v>2</v>
       </c>
-      <c r="C200" s="2" t="s">
-        <v>654</v>
+      <c r="C200" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="15" customHeight="1">
@@ -10072,11 +10119,11 @@
       <c r="B201" s="2">
         <v>3</v>
       </c>
-      <c r="C201" s="2" t="s">
-        <v>654</v>
+      <c r="C201" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="202" spans="1:4" ht="15" customHeight="1">
@@ -10086,11 +10133,11 @@
       <c r="B202" s="2">
         <v>0</v>
       </c>
-      <c r="C202" s="2" t="s">
-        <v>654</v>
+      <c r="C202" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="15" customHeight="1">
@@ -10100,11 +10147,11 @@
       <c r="B203" s="2">
         <v>1</v>
       </c>
-      <c r="C203" s="2" t="s">
-        <v>654</v>
+      <c r="C203" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="204" spans="1:4" ht="15" customHeight="1">
@@ -10114,11 +10161,11 @@
       <c r="B204" s="2">
         <v>0</v>
       </c>
-      <c r="C204" s="2" t="s">
-        <v>654</v>
+      <c r="C204" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15" customHeight="1">
@@ -10128,11 +10175,11 @@
       <c r="B205" s="2">
         <v>1</v>
       </c>
-      <c r="C205" s="2" t="s">
-        <v>654</v>
+      <c r="C205" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15" customHeight="1">
@@ -10142,11 +10189,11 @@
       <c r="B206" s="2">
         <v>0</v>
       </c>
-      <c r="C206" s="2" t="s">
-        <v>654</v>
+      <c r="C206" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="15" customHeight="1">
@@ -10156,11 +10203,11 @@
       <c r="B207" s="2">
         <v>1</v>
       </c>
-      <c r="C207" s="2" t="s">
-        <v>654</v>
+      <c r="C207" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15" customHeight="1">
@@ -10170,11 +10217,11 @@
       <c r="B208" s="2">
         <v>1</v>
       </c>
-      <c r="C208" s="2" t="s">
-        <v>654</v>
+      <c r="C208" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="15" customHeight="1">
@@ -10184,11 +10231,11 @@
       <c r="B209" s="2">
         <v>2</v>
       </c>
-      <c r="C209" s="2" t="s">
-        <v>654</v>
+      <c r="C209" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15" customHeight="1">
@@ -10198,11 +10245,11 @@
       <c r="B210" s="2">
         <v>3</v>
       </c>
-      <c r="C210" s="2" t="s">
-        <v>654</v>
+      <c r="C210" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15" customHeight="1">
@@ -10212,11 +10259,11 @@
       <c r="B211" s="2">
         <v>4</v>
       </c>
-      <c r="C211" s="2" t="s">
-        <v>654</v>
+      <c r="C211" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="15" customHeight="1">
@@ -10226,11 +10273,11 @@
       <c r="B212" s="2">
         <v>5</v>
       </c>
-      <c r="C212" s="2" t="s">
-        <v>654</v>
+      <c r="C212" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15" customHeight="1">
@@ -10240,11 +10287,11 @@
       <c r="B213" s="2">
         <v>0</v>
       </c>
-      <c r="C213" s="2" t="s">
-        <v>654</v>
+      <c r="C213" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15" customHeight="1">
@@ -10254,11 +10301,11 @@
       <c r="B214" s="2">
         <v>1</v>
       </c>
-      <c r="C214" s="2" t="s">
-        <v>654</v>
+      <c r="C214" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="215" spans="1:4" ht="15" customHeight="1">
@@ -10268,11 +10315,11 @@
       <c r="B215" s="2">
         <v>0</v>
       </c>
-      <c r="C215" s="2" t="s">
-        <v>654</v>
+      <c r="C215" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="216" spans="1:4" ht="15" customHeight="1">
@@ -10282,11 +10329,11 @@
       <c r="B216" s="2">
         <v>1</v>
       </c>
-      <c r="C216" s="2" t="s">
-        <v>654</v>
+      <c r="C216" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="217" spans="1:4" ht="15" customHeight="1">
@@ -10296,11 +10343,11 @@
       <c r="B217" s="2">
         <v>1</v>
       </c>
-      <c r="C217" s="2" t="s">
-        <v>654</v>
+      <c r="C217" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="218" spans="1:4" ht="15" customHeight="1">
@@ -10310,11 +10357,11 @@
       <c r="B218" s="2">
         <v>2</v>
       </c>
-      <c r="C218" s="2" t="s">
-        <v>654</v>
+      <c r="C218" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="219" spans="1:4" ht="15" customHeight="1">
@@ -10324,11 +10371,11 @@
       <c r="B219" s="2">
         <v>3</v>
       </c>
-      <c r="C219" s="2" t="s">
-        <v>654</v>
+      <c r="C219" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="15" customHeight="1">
@@ -10338,11 +10385,11 @@
       <c r="B220" s="2">
         <v>4</v>
       </c>
-      <c r="C220" s="2" t="s">
-        <v>654</v>
+      <c r="C220" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="221" spans="1:4" ht="15" customHeight="1">
@@ -10352,11 +10399,11 @@
       <c r="B221" s="2">
         <v>5</v>
       </c>
-      <c r="C221" s="2" t="s">
-        <v>654</v>
+      <c r="C221" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15" customHeight="1">
@@ -10366,11 +10413,11 @@
       <c r="B222" s="2">
         <v>1</v>
       </c>
-      <c r="C222" s="2" t="s">
-        <v>654</v>
+      <c r="C222" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="223" spans="1:4" ht="15" customHeight="1">
@@ -10380,11 +10427,11 @@
       <c r="B223" s="2">
         <v>2</v>
       </c>
-      <c r="C223" s="2" t="s">
-        <v>654</v>
+      <c r="C223" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="224" spans="1:4" ht="15" customHeight="1">
@@ -10394,11 +10441,11 @@
       <c r="B224" s="2">
         <v>3</v>
       </c>
-      <c r="C224" s="2" t="s">
-        <v>654</v>
+      <c r="C224" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="225" spans="1:4" ht="15" customHeight="1">
@@ -10408,11 +10455,11 @@
       <c r="B225" s="2">
         <v>4</v>
       </c>
-      <c r="C225" s="2" t="s">
-        <v>654</v>
+      <c r="C225" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="15" customHeight="1">
@@ -10422,11 +10469,11 @@
       <c r="B226" s="2">
         <v>5</v>
       </c>
-      <c r="C226" s="2" t="s">
-        <v>654</v>
+      <c r="C226" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="227" spans="1:4" ht="15" customHeight="1">
@@ -10436,11 +10483,11 @@
       <c r="B227" s="2">
         <v>0</v>
       </c>
-      <c r="C227" s="2" t="s">
-        <v>654</v>
+      <c r="C227" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15" customHeight="1">
@@ -10450,11 +10497,11 @@
       <c r="B228" s="2">
         <v>1</v>
       </c>
-      <c r="C228" s="2" t="s">
-        <v>654</v>
+      <c r="C228" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="229" spans="1:4" ht="15" customHeight="1">
@@ -10464,11 +10511,11 @@
       <c r="B229" s="2">
         <v>2</v>
       </c>
-      <c r="C229" s="2" t="s">
-        <v>654</v>
+      <c r="C229" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="230" spans="1:4" ht="15" customHeight="1">
@@ -10478,11 +10525,11 @@
       <c r="B230" s="2">
         <v>3</v>
       </c>
-      <c r="C230" s="2" t="s">
-        <v>654</v>
+      <c r="C230" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="15" customHeight="1">
@@ -10492,11 +10539,11 @@
       <c r="B231" s="2">
         <v>4</v>
       </c>
-      <c r="C231" s="2" t="s">
-        <v>654</v>
+      <c r="C231" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="232" spans="1:4" ht="15" customHeight="1">
@@ -10506,11 +10553,11 @@
       <c r="B232" s="2">
         <v>5</v>
       </c>
-      <c r="C232" s="2" t="s">
-        <v>654</v>
+      <c r="C232" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15" customHeight="1">
@@ -10520,11 +10567,11 @@
       <c r="B233" s="2">
         <v>6</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>654</v>
+      <c r="C233" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="234" spans="1:4" ht="15" customHeight="1">
@@ -10534,11 +10581,11 @@
       <c r="B234" s="2">
         <v>7</v>
       </c>
-      <c r="C234" s="2" t="s">
-        <v>654</v>
+      <c r="C234" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="235" spans="1:4" ht="15" customHeight="1">
@@ -10548,11 +10595,11 @@
       <c r="B235" s="2">
         <v>8</v>
       </c>
-      <c r="C235" s="2" t="s">
-        <v>654</v>
+      <c r="C235" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15" customHeight="1">
@@ -10562,11 +10609,11 @@
       <c r="B236" s="2">
         <v>9</v>
       </c>
-      <c r="C236" s="2" t="s">
-        <v>654</v>
+      <c r="C236" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15" customHeight="1">
@@ -10576,11 +10623,11 @@
       <c r="B237" s="2">
         <v>0</v>
       </c>
-      <c r="C237" s="2" t="s">
-        <v>654</v>
+      <c r="C237" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15" customHeight="1">
@@ -10590,11 +10637,11 @@
       <c r="B238" s="2">
         <v>1</v>
       </c>
-      <c r="C238" s="2" t="s">
-        <v>654</v>
+      <c r="C238" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="239" spans="1:4" ht="15" customHeight="1">
@@ -10604,11 +10651,11 @@
       <c r="B239" s="2">
         <v>2</v>
       </c>
-      <c r="C239" s="2" t="s">
-        <v>654</v>
+      <c r="C239" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="240" spans="1:4" ht="15" customHeight="1">
@@ -10618,11 +10665,11 @@
       <c r="B240" s="2">
         <v>3</v>
       </c>
-      <c r="C240" s="2" t="s">
-        <v>654</v>
+      <c r="C240" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="241" spans="1:4" ht="15" customHeight="1">
@@ -10632,11 +10679,11 @@
       <c r="B241" s="2">
         <v>4</v>
       </c>
-      <c r="C241" s="2" t="s">
-        <v>654</v>
+      <c r="C241" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="242" spans="1:4" ht="15" customHeight="1">
@@ -10646,11 +10693,11 @@
       <c r="B242" s="2">
         <v>5</v>
       </c>
-      <c r="C242" s="2" t="s">
-        <v>654</v>
+      <c r="C242" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="243" spans="1:4" ht="15" customHeight="1">
@@ -10660,11 +10707,11 @@
       <c r="B243" s="2">
         <v>6</v>
       </c>
-      <c r="C243" s="2" t="s">
-        <v>654</v>
+      <c r="C243" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="244" spans="1:4" ht="15" customHeight="1">
@@ -10674,11 +10721,11 @@
       <c r="B244" s="2">
         <v>7</v>
       </c>
-      <c r="C244" s="2" t="s">
-        <v>654</v>
+      <c r="C244" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D244" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="15" customHeight="1">
@@ -10688,11 +10735,11 @@
       <c r="B245" s="2">
         <v>8</v>
       </c>
-      <c r="C245" s="2" t="s">
-        <v>654</v>
+      <c r="C245" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D245" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1">
@@ -10702,11 +10749,11 @@
       <c r="B246" s="2">
         <v>9</v>
       </c>
-      <c r="C246" s="2" t="s">
-        <v>654</v>
+      <c r="C246" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15" customHeight="1">
@@ -10716,11 +10763,11 @@
       <c r="B247" s="2">
         <v>1001</v>
       </c>
-      <c r="C247" s="2" t="s">
-        <v>654</v>
+      <c r="C247" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D247" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15" customHeight="1">
@@ -10730,11 +10777,11 @@
       <c r="B248" s="2">
         <v>1102</v>
       </c>
-      <c r="C248" s="2" t="s">
-        <v>654</v>
+      <c r="C248" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15" customHeight="1">
@@ -10744,11 +10791,11 @@
       <c r="B249" s="2">
         <v>1103</v>
       </c>
-      <c r="C249" s="2" t="s">
-        <v>654</v>
+      <c r="C249" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D249" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15" customHeight="1">
@@ -10758,11 +10805,11 @@
       <c r="B250" s="2">
         <v>1104</v>
       </c>
-      <c r="C250" s="2" t="s">
-        <v>654</v>
+      <c r="C250" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15" customHeight="1">
@@ -10772,11 +10819,11 @@
       <c r="B251" s="2">
         <v>1201</v>
       </c>
-      <c r="C251" s="2" t="s">
-        <v>654</v>
+      <c r="C251" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1">
@@ -10786,11 +10833,11 @@
       <c r="B252" s="2">
         <v>1202</v>
       </c>
-      <c r="C252" s="2" t="s">
-        <v>654</v>
+      <c r="C252" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15" customHeight="1">
@@ -10800,11 +10847,11 @@
       <c r="B253" s="2">
         <v>1203</v>
       </c>
-      <c r="C253" s="2" t="s">
-        <v>654</v>
+      <c r="C253" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="254" spans="1:4" ht="15" customHeight="1">
@@ -10814,11 +10861,11 @@
       <c r="B254" s="2">
         <v>1301</v>
       </c>
-      <c r="C254" s="2" t="s">
-        <v>654</v>
+      <c r="C254" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15" customHeight="1">
@@ -10828,11 +10875,11 @@
       <c r="B255" s="2">
         <v>1401</v>
       </c>
-      <c r="C255" s="2" t="s">
-        <v>654</v>
+      <c r="C255" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15" customHeight="1">
@@ -10842,11 +10889,11 @@
       <c r="B256" s="2">
         <v>1501</v>
       </c>
-      <c r="C256" s="2" t="s">
-        <v>654</v>
+      <c r="C256" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1">
@@ -10856,11 +10903,11 @@
       <c r="B257" s="2">
         <v>1601</v>
       </c>
-      <c r="C257" s="2" t="s">
-        <v>654</v>
+      <c r="C257" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15" customHeight="1">
@@ -10870,11 +10917,11 @@
       <c r="B258" s="2">
         <v>1701</v>
       </c>
-      <c r="C258" s="2" t="s">
-        <v>654</v>
+      <c r="C258" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1">
@@ -10884,11 +10931,11 @@
       <c r="B259" s="2">
         <v>1801</v>
       </c>
-      <c r="C259" s="2" t="s">
-        <v>654</v>
+      <c r="C259" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="260" spans="1:4" ht="15" customHeight="1">
@@ -10898,11 +10945,11 @@
       <c r="B260" s="2">
         <v>1802</v>
       </c>
-      <c r="C260" s="2" t="s">
-        <v>654</v>
+      <c r="C260" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="261" spans="1:4" ht="15" customHeight="1">
@@ -10912,11 +10959,11 @@
       <c r="B261" s="2">
         <v>1901</v>
       </c>
-      <c r="C261" s="2" t="s">
-        <v>654</v>
+      <c r="C261" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="262" spans="1:4" ht="15" customHeight="1">
@@ -10926,11 +10973,11 @@
       <c r="B262" s="2">
         <v>2001</v>
       </c>
-      <c r="C262" s="2" t="s">
-        <v>654</v>
+      <c r="C262" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="263" spans="1:4" ht="15" customHeight="1">
@@ -10940,11 +10987,11 @@
       <c r="B263" s="2">
         <v>1</v>
       </c>
-      <c r="C263" s="2" t="s">
-        <v>654</v>
+      <c r="C263" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="264" spans="1:4" ht="15" customHeight="1">
@@ -10954,11 +11001,11 @@
       <c r="B264" s="2">
         <v>0</v>
       </c>
-      <c r="C264" s="2" t="s">
-        <v>654</v>
+      <c r="C264" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="265" spans="1:4" ht="15" customHeight="1">
@@ -10968,11 +11015,11 @@
       <c r="B265" s="2">
         <v>1</v>
       </c>
-      <c r="C265" s="2" t="s">
-        <v>654</v>
+      <c r="C265" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="266" spans="1:4" ht="15" customHeight="1">
@@ -10982,11 +11029,11 @@
       <c r="B266" s="2">
         <v>0</v>
       </c>
-      <c r="C266" s="2" t="s">
-        <v>654</v>
+      <c r="C266" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="267" spans="1:4" ht="15" customHeight="1">
@@ -10996,11 +11043,11 @@
       <c r="B267" s="2">
         <v>1</v>
       </c>
-      <c r="C267" s="2" t="s">
-        <v>654</v>
+      <c r="C267" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="268" spans="1:4" ht="15" customHeight="1">
@@ -11010,11 +11057,11 @@
       <c r="B268" s="2">
         <v>2</v>
       </c>
-      <c r="C268" s="2" t="s">
-        <v>654</v>
+      <c r="C268" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="269" spans="1:4" ht="15" customHeight="1">
@@ -11024,11 +11071,11 @@
       <c r="B269" s="2">
         <v>3</v>
       </c>
-      <c r="C269" s="2" t="s">
-        <v>654</v>
+      <c r="C269" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="270" spans="1:4" ht="15" customHeight="1">
@@ -11038,11 +11085,11 @@
       <c r="B270" s="2">
         <v>4</v>
       </c>
-      <c r="C270" s="2" t="s">
-        <v>654</v>
+      <c r="C270" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="271" spans="1:4" ht="15" customHeight="1">
@@ -11052,11 +11099,11 @@
       <c r="B271" s="2">
         <v>5</v>
       </c>
-      <c r="C271" s="2" t="s">
-        <v>654</v>
+      <c r="C271" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="272" spans="1:4" ht="15" customHeight="1">
@@ -11066,11 +11113,11 @@
       <c r="B272" s="2">
         <v>6</v>
       </c>
-      <c r="C272" s="2" t="s">
-        <v>654</v>
+      <c r="C272" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="273" spans="1:4" ht="15" customHeight="1">
@@ -11080,11 +11127,11 @@
       <c r="B273" s="2">
         <v>1</v>
       </c>
-      <c r="C273" s="2" t="s">
-        <v>654</v>
+      <c r="C273" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="274" spans="1:4" ht="15" customHeight="1">
@@ -11094,11 +11141,11 @@
       <c r="B274" s="2">
         <v>2</v>
       </c>
-      <c r="C274" s="2" t="s">
-        <v>654</v>
+      <c r="C274" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="275" spans="1:4" ht="15" customHeight="1">
@@ -11108,11 +11155,11 @@
       <c r="B275" s="2">
         <v>3</v>
       </c>
-      <c r="C275" s="2" t="s">
-        <v>654</v>
+      <c r="C275" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="276" spans="1:4" ht="15" customHeight="1">
@@ -11122,11 +11169,11 @@
       <c r="B276" s="2">
         <v>4</v>
       </c>
-      <c r="C276" s="2" t="s">
-        <v>654</v>
+      <c r="C276" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="277" spans="1:4" ht="15" customHeight="1">
@@ -11136,11 +11183,11 @@
       <c r="B277" s="2">
         <v>5</v>
       </c>
-      <c r="C277" s="2" t="s">
-        <v>654</v>
+      <c r="C277" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="278" spans="1:4" ht="15" customHeight="1">
@@ -11150,11 +11197,11 @@
       <c r="B278" s="2">
         <v>6</v>
       </c>
-      <c r="C278" s="2" t="s">
-        <v>654</v>
+      <c r="C278" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="279" spans="1:4" ht="15" customHeight="1">
@@ -11164,11 +11211,11 @@
       <c r="B279" s="2">
         <v>1</v>
       </c>
-      <c r="C279" s="2" t="s">
-        <v>654</v>
+      <c r="C279" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D279" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="280" spans="1:4" ht="15" customHeight="1">
@@ -11178,11 +11225,11 @@
       <c r="B280" s="2">
         <v>2</v>
       </c>
-      <c r="C280" s="2" t="s">
-        <v>654</v>
+      <c r="C280" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="281" spans="1:4" ht="15" customHeight="1">
@@ -11192,11 +11239,11 @@
       <c r="B281" s="2">
         <v>3</v>
       </c>
-      <c r="C281" s="2" t="s">
-        <v>654</v>
+      <c r="C281" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="282" spans="1:4" ht="15" customHeight="1">
@@ -11206,11 +11253,11 @@
       <c r="B282" s="2">
         <v>1</v>
       </c>
-      <c r="C282" s="2" t="s">
-        <v>654</v>
+      <c r="C282" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="15" customHeight="1">
@@ -11220,11 +11267,11 @@
       <c r="B283" s="2">
         <v>2</v>
       </c>
-      <c r="C283" s="2" t="s">
-        <v>654</v>
+      <c r="C283" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="15" customHeight="1">
@@ -11234,11 +11281,11 @@
       <c r="B284" s="2">
         <v>3</v>
       </c>
-      <c r="C284" s="2" t="s">
-        <v>654</v>
+      <c r="C284" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15" customHeight="1">
@@ -11248,11 +11295,11 @@
       <c r="B285" s="2">
         <v>4</v>
       </c>
-      <c r="C285" s="2" t="s">
-        <v>654</v>
+      <c r="C285" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="15" customHeight="1">
@@ -11262,11 +11309,11 @@
       <c r="B286" s="2">
         <v>5</v>
       </c>
-      <c r="C286" s="2" t="s">
-        <v>654</v>
+      <c r="C286" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15" customHeight="1">
@@ -11276,11 +11323,11 @@
       <c r="B287" s="2">
         <v>1</v>
       </c>
-      <c r="C287" s="2" t="s">
-        <v>654</v>
+      <c r="C287" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="15" customHeight="1">
@@ -11290,11 +11337,11 @@
       <c r="B288" s="2">
         <v>2</v>
       </c>
-      <c r="C288" s="2" t="s">
-        <v>654</v>
+      <c r="C288" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="289" spans="1:4" ht="15" customHeight="1">
@@ -11304,11 +11351,11 @@
       <c r="B289" s="2">
         <v>3</v>
       </c>
-      <c r="C289" s="2" t="s">
-        <v>654</v>
+      <c r="C289" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="290" spans="1:4" ht="15" customHeight="1">
@@ -11318,11 +11365,11 @@
       <c r="B290" s="2">
         <v>1</v>
       </c>
-      <c r="C290" s="2" t="s">
-        <v>654</v>
+      <c r="C290" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="291" spans="1:4" ht="15" customHeight="1">
@@ -11332,11 +11379,11 @@
       <c r="B291" s="2">
         <v>2</v>
       </c>
-      <c r="C291" s="2" t="s">
-        <v>654</v>
+      <c r="C291" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15" customHeight="1">
@@ -11346,11 +11393,11 @@
       <c r="B292" s="2">
         <v>3</v>
       </c>
-      <c r="C292" s="2" t="s">
-        <v>654</v>
+      <c r="C292" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="15" customHeight="1">
@@ -11360,11 +11407,11 @@
       <c r="B293" s="2">
         <v>1</v>
       </c>
-      <c r="C293" s="2" t="s">
-        <v>654</v>
+      <c r="C293" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="294" spans="1:4" ht="15" customHeight="1">
@@ -11374,11 +11421,11 @@
       <c r="B294" s="2">
         <v>2</v>
       </c>
-      <c r="C294" s="2" t="s">
-        <v>654</v>
+      <c r="C294" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="295" spans="1:4" ht="15" customHeight="1">
@@ -11388,11 +11435,11 @@
       <c r="B295" s="2">
         <v>3</v>
       </c>
-      <c r="C295" s="2" t="s">
-        <v>654</v>
+      <c r="C295" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="296" spans="1:4" ht="15" customHeight="1">
@@ -11402,11 +11449,11 @@
       <c r="B296" s="2">
         <v>0</v>
       </c>
-      <c r="C296" s="2" t="s">
-        <v>654</v>
+      <c r="C296" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="297" spans="1:4" ht="15" customHeight="1">
@@ -11416,11 +11463,11 @@
       <c r="B297" s="2">
         <v>1</v>
       </c>
-      <c r="C297" s="2" t="s">
-        <v>654</v>
+      <c r="C297" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="298" spans="1:4" ht="15" customHeight="1">
@@ -11430,11 +11477,11 @@
       <c r="B298" s="2">
         <v>0</v>
       </c>
-      <c r="C298" s="2" t="s">
-        <v>654</v>
+      <c r="C298" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D298" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15" customHeight="1">
@@ -11444,11 +11491,11 @@
       <c r="B299" s="2">
         <v>1</v>
       </c>
-      <c r="C299" s="2" t="s">
-        <v>654</v>
+      <c r="C299" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="300" spans="1:4" ht="15" customHeight="1">
@@ -11458,11 +11505,11 @@
       <c r="B300" s="2">
         <v>0</v>
       </c>
-      <c r="C300" s="2" t="s">
-        <v>654</v>
+      <c r="C300" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15" customHeight="1">
@@ -11472,11 +11519,11 @@
       <c r="B301" s="2">
         <v>1</v>
       </c>
-      <c r="C301" s="2" t="s">
-        <v>654</v>
+      <c r="C301" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix quarterly variables and updated categories to FALSE
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0987AAF-69E2-FA4C-B363-04986BB79F39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16160" windowHeight="10240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="16164" windowHeight="10236" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2156" uniqueCount="818">
   <si>
     <t>name</t>
   </si>
@@ -2472,12 +2466,15 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -2552,8 +2549,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2569,7 +2566,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2611,7 +2608,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2643,27 +2640,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2695,24 +2674,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2888,20 +2849,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D313"/>
   <sheetViews>
     <sheetView topLeftCell="A283" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="197.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="197.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -7295,21 +7256,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D299" sqref="D299"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -7333,8 +7294,8 @@
       <c r="B2" s="2">
         <v>101</v>
       </c>
-      <c r="C2" s="2" t="b">
-        <v>0</v>
+      <c r="C2" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>654</v>
@@ -7347,8 +7308,8 @@
       <c r="B3" s="2">
         <v>102</v>
       </c>
-      <c r="C3" s="2" t="b">
-        <v>0</v>
+      <c r="C3" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>655</v>
@@ -7361,8 +7322,8 @@
       <c r="B4" s="2">
         <v>103</v>
       </c>
-      <c r="C4" s="2" t="b">
-        <v>0</v>
+      <c r="C4" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>656</v>
@@ -7375,8 +7336,8 @@
       <c r="B5" s="2">
         <v>104</v>
       </c>
-      <c r="C5" s="2" t="b">
-        <v>0</v>
+      <c r="C5" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>657</v>
@@ -7389,8 +7350,8 @@
       <c r="B6" s="2">
         <v>105</v>
       </c>
-      <c r="C6" s="2" t="b">
-        <v>0</v>
+      <c r="C6" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>658</v>
@@ -7403,8 +7364,8 @@
       <c r="B7" s="2">
         <v>106</v>
       </c>
-      <c r="C7" s="2" t="b">
-        <v>0</v>
+      <c r="C7" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>659</v>
@@ -7417,8 +7378,8 @@
       <c r="B8" s="2">
         <v>107</v>
       </c>
-      <c r="C8" s="2" t="b">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>660</v>
@@ -7431,8 +7392,8 @@
       <c r="B9" s="2">
         <v>108</v>
       </c>
-      <c r="C9" s="2" t="b">
-        <v>0</v>
+      <c r="C9" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>661</v>
@@ -7445,8 +7406,8 @@
       <c r="B10" s="2">
         <v>109</v>
       </c>
-      <c r="C10" s="2" t="b">
-        <v>0</v>
+      <c r="C10" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>662</v>
@@ -7459,8 +7420,8 @@
       <c r="B11" s="2">
         <v>110</v>
       </c>
-      <c r="C11" s="2" t="b">
-        <v>0</v>
+      <c r="C11" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>663</v>
@@ -7473,8 +7434,8 @@
       <c r="B12" s="2">
         <v>111</v>
       </c>
-      <c r="C12" s="2" t="b">
-        <v>0</v>
+      <c r="C12" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>664</v>
@@ -7487,8 +7448,8 @@
       <c r="B13" s="2">
         <v>112</v>
       </c>
-      <c r="C13" s="2" t="b">
-        <v>0</v>
+      <c r="C13" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>665</v>
@@ -7501,8 +7462,8 @@
       <c r="B14" s="2">
         <v>113</v>
       </c>
-      <c r="C14" s="2" t="b">
-        <v>0</v>
+      <c r="C14" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>666</v>
@@ -7515,8 +7476,8 @@
       <c r="B15" s="2">
         <v>114</v>
       </c>
-      <c r="C15" s="2" t="b">
-        <v>0</v>
+      <c r="C15" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>667</v>
@@ -7529,8 +7490,8 @@
       <c r="B16" s="2">
         <v>115</v>
       </c>
-      <c r="C16" s="2" t="b">
-        <v>0</v>
+      <c r="C16" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>668</v>
@@ -7543,8 +7504,8 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="2" t="b">
-        <v>0</v>
+      <c r="C17" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>669</v>
@@ -7557,8 +7518,8 @@
       <c r="B18" s="2">
         <v>117</v>
       </c>
-      <c r="C18" s="2" t="b">
-        <v>0</v>
+      <c r="C18" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>670</v>
@@ -7571,8 +7532,8 @@
       <c r="B19" s="2">
         <v>118</v>
       </c>
-      <c r="C19" s="2" t="b">
-        <v>0</v>
+      <c r="C19" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>671</v>
@@ -7585,8 +7546,8 @@
       <c r="B20" s="2">
         <v>119</v>
       </c>
-      <c r="C20" s="2" t="b">
-        <v>0</v>
+      <c r="C20" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>672</v>
@@ -7599,8 +7560,8 @@
       <c r="B21" s="2">
         <v>120</v>
       </c>
-      <c r="C21" s="2" t="b">
-        <v>0</v>
+      <c r="C21" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>673</v>
@@ -7613,8 +7574,8 @@
       <c r="B22" s="2">
         <v>121</v>
       </c>
-      <c r="C22" s="2" t="b">
-        <v>0</v>
+      <c r="C22" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>674</v>
@@ -7627,8 +7588,8 @@
       <c r="B23" s="2">
         <v>122</v>
       </c>
-      <c r="C23" s="2" t="b">
-        <v>0</v>
+      <c r="C23" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>675</v>
@@ -7641,8 +7602,8 @@
       <c r="B24" s="2">
         <v>36</v>
       </c>
-      <c r="C24" s="2" t="b">
-        <v>0</v>
+      <c r="C24" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>676</v>
@@ -7655,8 +7616,8 @@
       <c r="B25" s="2">
         <v>208</v>
       </c>
-      <c r="C25" s="2" t="b">
-        <v>0</v>
+      <c r="C25" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>677</v>
@@ -7669,8 +7630,8 @@
       <c r="B26" s="2">
         <v>246</v>
       </c>
-      <c r="C26" s="2" t="b">
-        <v>0</v>
+      <c r="C26" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>678</v>
@@ -7683,8 +7644,8 @@
       <c r="B27" s="2">
         <v>250</v>
       </c>
-      <c r="C27" s="2" t="b">
-        <v>0</v>
+      <c r="C27" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>679</v>
@@ -7697,8 +7658,8 @@
       <c r="B28" s="2">
         <v>276</v>
       </c>
-      <c r="C28" s="2" t="b">
-        <v>0</v>
+      <c r="C28" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>680</v>
@@ -7711,8 +7672,8 @@
       <c r="B29" s="2">
         <v>300</v>
       </c>
-      <c r="C29" s="2" t="b">
-        <v>0</v>
+      <c r="C29" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>681</v>
@@ -7725,8 +7686,8 @@
       <c r="B30" s="2">
         <v>380</v>
       </c>
-      <c r="C30" s="2" t="b">
-        <v>0</v>
+      <c r="C30" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>682</v>
@@ -7739,8 +7700,8 @@
       <c r="B31" s="2">
         <v>528</v>
       </c>
-      <c r="C31" s="2" t="b">
-        <v>0</v>
+      <c r="C31" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>683</v>
@@ -7753,8 +7714,8 @@
       <c r="B32" s="2">
         <v>578</v>
       </c>
-      <c r="C32" s="2" t="b">
-        <v>0</v>
+      <c r="C32" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>684</v>
@@ -7767,8 +7728,8 @@
       <c r="B33" s="2">
         <v>724</v>
       </c>
-      <c r="C33" s="2" t="b">
-        <v>0</v>
+      <c r="C33" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>685</v>
@@ -7781,8 +7742,8 @@
       <c r="B34" s="2">
         <v>826</v>
       </c>
-      <c r="C34" s="2" t="b">
-        <v>0</v>
+      <c r="C34" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>686</v>
@@ -7795,8 +7756,8 @@
       <c r="B35" s="2">
         <v>0</v>
       </c>
-      <c r="C35" s="2" t="b">
-        <v>0</v>
+      <c r="C35" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>687</v>
@@ -7809,8 +7770,8 @@
       <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="2" t="b">
-        <v>0</v>
+      <c r="C36" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>688</v>
@@ -7823,8 +7784,8 @@
       <c r="B37" s="2">
         <v>2</v>
       </c>
-      <c r="C37" s="2" t="b">
-        <v>0</v>
+      <c r="C37" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>689</v>
@@ -7837,8 +7798,8 @@
       <c r="B38" s="2">
         <v>1</v>
       </c>
-      <c r="C38" s="2" t="b">
-        <v>0</v>
+      <c r="C38" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>690</v>
@@ -7851,8 +7812,8 @@
       <c r="B39" s="2">
         <v>2</v>
       </c>
-      <c r="C39" s="2" t="b">
-        <v>0</v>
+      <c r="C39" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>691</v>
@@ -7865,8 +7826,8 @@
       <c r="B40" s="2">
         <v>3</v>
       </c>
-      <c r="C40" s="2" t="b">
-        <v>0</v>
+      <c r="C40" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>692</v>
@@ -7879,8 +7840,8 @@
       <c r="B41" s="2">
         <v>1</v>
       </c>
-      <c r="C41" s="2" t="b">
-        <v>0</v>
+      <c r="C41" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>693</v>
@@ -7893,8 +7854,8 @@
       <c r="B42" s="2">
         <v>2</v>
       </c>
-      <c r="C42" s="2" t="b">
-        <v>0</v>
+      <c r="C42" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>694</v>
@@ -7907,8 +7868,8 @@
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="2" t="b">
-        <v>0</v>
+      <c r="C43" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>692</v>
@@ -7921,8 +7882,8 @@
       <c r="B44" s="2">
         <v>1</v>
       </c>
-      <c r="C44" s="2" t="b">
-        <v>0</v>
+      <c r="C44" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>690</v>
@@ -7935,8 +7896,8 @@
       <c r="B45" s="2">
         <v>2</v>
       </c>
-      <c r="C45" s="2" t="b">
-        <v>0</v>
+      <c r="C45" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>691</v>
@@ -7949,8 +7910,8 @@
       <c r="B46" s="2">
         <v>3</v>
       </c>
-      <c r="C46" s="2" t="b">
-        <v>0</v>
+      <c r="C46" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>692</v>
@@ -7963,8 +7924,8 @@
       <c r="B47" s="2">
         <v>0</v>
       </c>
-      <c r="C47" s="2" t="b">
-        <v>0</v>
+      <c r="C47" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>695</v>
@@ -7977,8 +7938,8 @@
       <c r="B48" s="2">
         <v>1</v>
       </c>
-      <c r="C48" s="2" t="b">
-        <v>0</v>
+      <c r="C48" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>696</v>
@@ -7991,8 +7952,8 @@
       <c r="B49" s="2">
         <v>0</v>
       </c>
-      <c r="C49" s="2" t="b">
-        <v>0</v>
+      <c r="C49" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>697</v>
@@ -8005,8 +7966,8 @@
       <c r="B50" s="2">
         <v>1</v>
       </c>
-      <c r="C50" s="2" t="b">
-        <v>0</v>
+      <c r="C50" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>698</v>
@@ -8019,8 +7980,8 @@
       <c r="B51" s="2">
         <v>0</v>
       </c>
-      <c r="C51" s="2" t="b">
-        <v>0</v>
+      <c r="C51" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>697</v>
@@ -8033,8 +7994,8 @@
       <c r="B52" s="2">
         <v>1</v>
       </c>
-      <c r="C52" s="2" t="b">
-        <v>0</v>
+      <c r="C52" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>698</v>
@@ -8047,8 +8008,8 @@
       <c r="B53" s="2">
         <v>0</v>
       </c>
-      <c r="C53" s="2" t="b">
-        <v>0</v>
+      <c r="C53" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>697</v>
@@ -8061,8 +8022,8 @@
       <c r="B54" s="2">
         <v>1</v>
       </c>
-      <c r="C54" s="2" t="b">
-        <v>0</v>
+      <c r="C54" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>698</v>
@@ -8075,8 +8036,8 @@
       <c r="B55" s="2">
         <v>2</v>
       </c>
-      <c r="C55" s="2" t="b">
-        <v>0</v>
+      <c r="C55" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>699</v>
@@ -8089,8 +8050,8 @@
       <c r="B56" s="2">
         <v>3</v>
       </c>
-      <c r="C56" s="2" t="b">
-        <v>0</v>
+      <c r="C56" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>700</v>
@@ -8103,8 +8064,8 @@
       <c r="B57" s="2">
         <v>0</v>
       </c>
-      <c r="C57" s="2" t="b">
-        <v>0</v>
+      <c r="C57" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>697</v>
@@ -8117,8 +8078,8 @@
       <c r="B58" s="2">
         <v>1</v>
       </c>
-      <c r="C58" s="2" t="b">
-        <v>0</v>
+      <c r="C58" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>698</v>
@@ -8131,8 +8092,8 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="2" t="b">
-        <v>0</v>
+      <c r="C59" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>695</v>
@@ -8145,8 +8106,8 @@
       <c r="B60" s="2">
         <v>2</v>
       </c>
-      <c r="C60" s="2" t="b">
-        <v>0</v>
+      <c r="C60" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>701</v>
@@ -8159,8 +8120,8 @@
       <c r="B61" s="2">
         <v>3</v>
       </c>
-      <c r="C61" s="2" t="b">
-        <v>0</v>
+      <c r="C61" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>702</v>
@@ -8173,8 +8134,8 @@
       <c r="B62" s="2">
         <v>4</v>
       </c>
-      <c r="C62" s="2" t="b">
-        <v>0</v>
+      <c r="C62" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>380</v>
@@ -8187,8 +8148,8 @@
       <c r="B63" s="2">
         <v>5</v>
       </c>
-      <c r="C63" s="2" t="b">
-        <v>0</v>
+      <c r="C63" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>703</v>
@@ -8201,8 +8162,8 @@
       <c r="B64" s="2">
         <v>0</v>
       </c>
-      <c r="C64" s="2" t="b">
-        <v>0</v>
+      <c r="C64" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>704</v>
@@ -8215,8 +8176,8 @@
       <c r="B65" s="2">
         <v>1</v>
       </c>
-      <c r="C65" s="2" t="b">
-        <v>0</v>
+      <c r="C65" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>705</v>
@@ -8229,8 +8190,8 @@
       <c r="B66" s="2">
         <v>0</v>
       </c>
-      <c r="C66" s="2" t="b">
-        <v>0</v>
+      <c r="C66" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>704</v>
@@ -8243,8 +8204,8 @@
       <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="C67" s="2" t="b">
-        <v>0</v>
+      <c r="C67" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>705</v>
@@ -8257,8 +8218,8 @@
       <c r="B68" s="2">
         <v>0</v>
       </c>
-      <c r="C68" s="2" t="b">
-        <v>0</v>
+      <c r="C68" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>704</v>
@@ -8271,8 +8232,8 @@
       <c r="B69" s="2">
         <v>1</v>
       </c>
-      <c r="C69" s="2" t="b">
-        <v>0</v>
+      <c r="C69" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>705</v>
@@ -8285,8 +8246,8 @@
       <c r="B70" s="2">
         <v>0</v>
       </c>
-      <c r="C70" s="2" t="b">
-        <v>0</v>
+      <c r="C70" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>704</v>
@@ -8299,8 +8260,8 @@
       <c r="B71" s="2">
         <v>1</v>
       </c>
-      <c r="C71" s="2" t="b">
-        <v>0</v>
+      <c r="C71" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>705</v>
@@ -8313,8 +8274,8 @@
       <c r="B72" s="2">
         <v>0</v>
       </c>
-      <c r="C72" s="2" t="b">
-        <v>0</v>
+      <c r="C72" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>704</v>
@@ -8327,8 +8288,8 @@
       <c r="B73" s="2">
         <v>1</v>
       </c>
-      <c r="C73" s="2" t="b">
-        <v>0</v>
+      <c r="C73" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>705</v>
@@ -8341,8 +8302,8 @@
       <c r="B74" s="2">
         <v>0</v>
       </c>
-      <c r="C74" s="2" t="b">
-        <v>0</v>
+      <c r="C74" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>704</v>
@@ -8355,8 +8316,8 @@
       <c r="B75" s="2">
         <v>1</v>
       </c>
-      <c r="C75" s="2" t="b">
-        <v>0</v>
+      <c r="C75" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>705</v>
@@ -8369,8 +8330,8 @@
       <c r="B76" s="2">
         <v>0</v>
       </c>
-      <c r="C76" s="2" t="b">
-        <v>0</v>
+      <c r="C76" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>704</v>
@@ -8383,8 +8344,8 @@
       <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C77" s="2" t="b">
-        <v>0</v>
+      <c r="C77" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>705</v>
@@ -8397,8 +8358,8 @@
       <c r="B78" s="2">
         <v>0</v>
       </c>
-      <c r="C78" s="2" t="b">
-        <v>0</v>
+      <c r="C78" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>704</v>
@@ -8411,8 +8372,8 @@
       <c r="B79" s="2">
         <v>1</v>
       </c>
-      <c r="C79" s="2" t="b">
-        <v>0</v>
+      <c r="C79" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>705</v>
@@ -8425,8 +8386,8 @@
       <c r="B80" s="2">
         <v>0</v>
       </c>
-      <c r="C80" s="2" t="b">
-        <v>0</v>
+      <c r="C80" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>704</v>
@@ -8439,8 +8400,8 @@
       <c r="B81" s="2">
         <v>1</v>
       </c>
-      <c r="C81" s="2" t="b">
-        <v>0</v>
+      <c r="C81" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>705</v>
@@ -8453,8 +8414,8 @@
       <c r="B82" s="2">
         <v>0</v>
       </c>
-      <c r="C82" s="2" t="b">
-        <v>0</v>
+      <c r="C82" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>704</v>
@@ -8467,8 +8428,8 @@
       <c r="B83" s="2">
         <v>1</v>
       </c>
-      <c r="C83" s="2" t="b">
-        <v>0</v>
+      <c r="C83" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>705</v>
@@ -8481,8 +8442,8 @@
       <c r="B84" s="2">
         <v>0</v>
       </c>
-      <c r="C84" s="2" t="b">
-        <v>0</v>
+      <c r="C84" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>706</v>
@@ -8495,8 +8456,8 @@
       <c r="B85" s="2">
         <v>1</v>
       </c>
-      <c r="C85" s="2" t="b">
-        <v>0</v>
+      <c r="C85" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>707</v>
@@ -8509,8 +8470,8 @@
       <c r="B86" s="2">
         <v>2</v>
       </c>
-      <c r="C86" s="2" t="b">
-        <v>0</v>
+      <c r="C86" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>708</v>
@@ -8523,8 +8484,8 @@
       <c r="B87" s="2">
         <v>0</v>
       </c>
-      <c r="C87" s="2" t="b">
-        <v>0</v>
+      <c r="C87" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>704</v>
@@ -8537,8 +8498,8 @@
       <c r="B88" s="2">
         <v>1</v>
       </c>
-      <c r="C88" s="2" t="b">
-        <v>0</v>
+      <c r="C88" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>705</v>
@@ -8551,8 +8512,8 @@
       <c r="B89" s="2">
         <v>0</v>
       </c>
-      <c r="C89" s="2" t="b">
-        <v>0</v>
+      <c r="C89" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>706</v>
@@ -8565,8 +8526,8 @@
       <c r="B90" s="2">
         <v>1</v>
       </c>
-      <c r="C90" s="2" t="b">
-        <v>0</v>
+      <c r="C90" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>707</v>
@@ -8579,8 +8540,8 @@
       <c r="B91" s="2">
         <v>2</v>
       </c>
-      <c r="C91" s="2" t="b">
-        <v>0</v>
+      <c r="C91" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>708</v>
@@ -8593,8 +8554,8 @@
       <c r="B92" s="2">
         <v>0</v>
       </c>
-      <c r="C92" s="2" t="b">
-        <v>0</v>
+      <c r="C92" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>704</v>
@@ -8607,8 +8568,8 @@
       <c r="B93" s="2">
         <v>1</v>
       </c>
-      <c r="C93" s="2" t="b">
-        <v>0</v>
+      <c r="C93" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>705</v>
@@ -8621,8 +8582,8 @@
       <c r="B94" s="2">
         <v>0</v>
       </c>
-      <c r="C94" s="2" t="b">
-        <v>0</v>
+      <c r="C94" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>709</v>
@@ -8635,8 +8596,8 @@
       <c r="B95" s="2">
         <v>1</v>
       </c>
-      <c r="C95" s="2" t="b">
-        <v>0</v>
+      <c r="C95" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>710</v>
@@ -8649,8 +8610,8 @@
       <c r="B96" s="2">
         <v>2</v>
       </c>
-      <c r="C96" s="2" t="b">
-        <v>0</v>
+      <c r="C96" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>711</v>
@@ -8663,8 +8624,8 @@
       <c r="B97" s="2">
         <v>3</v>
       </c>
-      <c r="C97" s="2" t="b">
-        <v>0</v>
+      <c r="C97" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>712</v>
@@ -8677,8 +8638,8 @@
       <c r="B98" s="2">
         <v>4</v>
       </c>
-      <c r="C98" s="2" t="b">
-        <v>0</v>
+      <c r="C98" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>713</v>
@@ -8691,8 +8652,8 @@
       <c r="B99" s="2">
         <v>0</v>
       </c>
-      <c r="C99" s="2" t="b">
-        <v>0</v>
+      <c r="C99" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>704</v>
@@ -8705,8 +8666,8 @@
       <c r="B100" s="2">
         <v>1</v>
       </c>
-      <c r="C100" s="2" t="b">
-        <v>0</v>
+      <c r="C100" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>705</v>
@@ -8719,8 +8680,8 @@
       <c r="B101" s="2">
         <v>0</v>
       </c>
-      <c r="C101" s="2" t="b">
-        <v>0</v>
+      <c r="C101" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>706</v>
@@ -8733,8 +8694,8 @@
       <c r="B102" s="2">
         <v>1</v>
       </c>
-      <c r="C102" s="2" t="b">
-        <v>0</v>
+      <c r="C102" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>714</v>
@@ -8747,8 +8708,8 @@
       <c r="B103" s="2">
         <v>2</v>
       </c>
-      <c r="C103" s="2" t="b">
-        <v>0</v>
+      <c r="C103" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>715</v>
@@ -8761,8 +8722,8 @@
       <c r="B104" s="2">
         <v>3</v>
       </c>
-      <c r="C104" s="2" t="b">
-        <v>0</v>
+      <c r="C104" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>716</v>
@@ -8775,8 +8736,8 @@
       <c r="B105" s="2">
         <v>0</v>
       </c>
-      <c r="C105" s="2" t="b">
-        <v>0</v>
+      <c r="C105" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>704</v>
@@ -8789,8 +8750,8 @@
       <c r="B106" s="2">
         <v>1</v>
       </c>
-      <c r="C106" s="2" t="b">
-        <v>0</v>
+      <c r="C106" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>705</v>
@@ -8803,8 +8764,8 @@
       <c r="B107" s="2">
         <v>0</v>
       </c>
-      <c r="C107" s="2" t="b">
-        <v>0</v>
+      <c r="C107" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>704</v>
@@ -8817,8 +8778,8 @@
       <c r="B108" s="2">
         <v>1</v>
       </c>
-      <c r="C108" s="2" t="b">
-        <v>0</v>
+      <c r="C108" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>705</v>
@@ -8831,8 +8792,8 @@
       <c r="B109" s="2">
         <v>0</v>
       </c>
-      <c r="C109" s="2" t="b">
-        <v>0</v>
+      <c r="C109" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>704</v>
@@ -8845,8 +8806,8 @@
       <c r="B110" s="2">
         <v>1</v>
       </c>
-      <c r="C110" s="2" t="b">
-        <v>0</v>
+      <c r="C110" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>705</v>
@@ -8859,8 +8820,8 @@
       <c r="B111" s="2">
         <v>0</v>
       </c>
-      <c r="C111" s="2" t="b">
-        <v>0</v>
+      <c r="C111" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>717</v>
@@ -8873,8 +8834,8 @@
       <c r="B112" s="2">
         <v>1</v>
       </c>
-      <c r="C112" s="2" t="b">
-        <v>0</v>
+      <c r="C112" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>718</v>
@@ -8887,8 +8848,8 @@
       <c r="B113" s="2">
         <v>2</v>
       </c>
-      <c r="C113" s="2" t="b">
-        <v>0</v>
+      <c r="C113" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>719</v>
@@ -8901,8 +8862,8 @@
       <c r="B114" s="2">
         <v>3</v>
       </c>
-      <c r="C114" s="2" t="b">
-        <v>0</v>
+      <c r="C114" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>720</v>
@@ -8915,8 +8876,8 @@
       <c r="B115" s="2">
         <v>4</v>
       </c>
-      <c r="C115" s="2" t="b">
-        <v>0</v>
+      <c r="C115" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>721</v>
@@ -8929,8 +8890,8 @@
       <c r="B116" s="2">
         <v>1</v>
       </c>
-      <c r="C116" s="2" t="b">
-        <v>0</v>
+      <c r="C116" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>722</v>
@@ -8943,8 +8904,8 @@
       <c r="B117" s="2">
         <v>2</v>
       </c>
-      <c r="C117" s="2" t="b">
-        <v>0</v>
+      <c r="C117" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>723</v>
@@ -8957,8 +8918,8 @@
       <c r="B118" s="2">
         <v>0</v>
       </c>
-      <c r="C118" s="2" t="b">
-        <v>0</v>
+      <c r="C118" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>704</v>
@@ -8971,8 +8932,8 @@
       <c r="B119" s="2">
         <v>1</v>
       </c>
-      <c r="C119" s="2" t="b">
-        <v>0</v>
+      <c r="C119" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>705</v>
@@ -8985,8 +8946,8 @@
       <c r="B120" s="2">
         <v>0</v>
       </c>
-      <c r="C120" s="2" t="b">
-        <v>0</v>
+      <c r="C120" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>704</v>
@@ -8999,8 +8960,8 @@
       <c r="B121" s="2">
         <v>1</v>
       </c>
-      <c r="C121" s="2" t="b">
-        <v>0</v>
+      <c r="C121" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>705</v>
@@ -9013,8 +8974,8 @@
       <c r="B122" s="2">
         <v>1</v>
       </c>
-      <c r="C122" s="2" t="b">
-        <v>0</v>
+      <c r="C122" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>724</v>
@@ -9027,8 +8988,8 @@
       <c r="B123" s="2">
         <v>2</v>
       </c>
-      <c r="C123" s="2" t="b">
-        <v>0</v>
+      <c r="C123" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>725</v>
@@ -9041,8 +9002,8 @@
       <c r="B124" s="2">
         <v>3</v>
       </c>
-      <c r="C124" s="2" t="b">
-        <v>0</v>
+      <c r="C124" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>726</v>
@@ -9055,8 +9016,8 @@
       <c r="B125" s="2">
         <v>4</v>
       </c>
-      <c r="C125" s="2" t="b">
-        <v>0</v>
+      <c r="C125" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>727</v>
@@ -9069,8 +9030,8 @@
       <c r="B126" s="2">
         <v>5</v>
       </c>
-      <c r="C126" s="2" t="b">
-        <v>0</v>
+      <c r="C126" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>728</v>
@@ -9083,8 +9044,8 @@
       <c r="B127" s="2">
         <v>6</v>
       </c>
-      <c r="C127" s="2" t="b">
-        <v>0</v>
+      <c r="C127" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>729</v>
@@ -9097,8 +9058,8 @@
       <c r="B128" s="2">
         <v>1</v>
       </c>
-      <c r="C128" s="2" t="b">
-        <v>0</v>
+      <c r="C128" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>730</v>
@@ -9111,8 +9072,8 @@
       <c r="B129" s="2">
         <v>2</v>
       </c>
-      <c r="C129" s="2" t="b">
-        <v>0</v>
+      <c r="C129" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>731</v>
@@ -9125,8 +9086,8 @@
       <c r="B130" s="2">
         <v>3</v>
       </c>
-      <c r="C130" s="2" t="b">
-        <v>0</v>
+      <c r="C130" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>732</v>
@@ -9139,8 +9100,8 @@
       <c r="B131" s="2">
         <v>4</v>
       </c>
-      <c r="C131" s="2" t="b">
-        <v>0</v>
+      <c r="C131" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>733</v>
@@ -9153,8 +9114,8 @@
       <c r="B132" s="2">
         <v>5</v>
       </c>
-      <c r="C132" s="2" t="b">
-        <v>0</v>
+      <c r="C132" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>734</v>
@@ -9167,8 +9128,8 @@
       <c r="B133" s="2">
         <v>0</v>
       </c>
-      <c r="C133" s="2" t="b">
-        <v>0</v>
+      <c r="C133" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>704</v>
@@ -9181,8 +9142,8 @@
       <c r="B134" s="2">
         <v>1</v>
       </c>
-      <c r="C134" s="2" t="b">
-        <v>0</v>
+      <c r="C134" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>705</v>
@@ -9195,8 +9156,8 @@
       <c r="B135" s="2">
         <v>0</v>
       </c>
-      <c r="C135" s="2" t="b">
-        <v>0</v>
+      <c r="C135" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>687</v>
@@ -9209,8 +9170,8 @@
       <c r="B136" s="2">
         <v>1</v>
       </c>
-      <c r="C136" s="2" t="b">
-        <v>0</v>
+      <c r="C136" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>688</v>
@@ -9223,8 +9184,8 @@
       <c r="B137" s="2">
         <v>2</v>
       </c>
-      <c r="C137" s="2" t="b">
-        <v>0</v>
+      <c r="C137" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>689</v>
@@ -9237,8 +9198,8 @@
       <c r="B138" s="2">
         <v>1</v>
       </c>
-      <c r="C138" s="2" t="b">
-        <v>0</v>
+      <c r="C138" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>735</v>
@@ -9251,8 +9212,8 @@
       <c r="B139" s="2">
         <v>2</v>
       </c>
-      <c r="C139" s="2" t="b">
-        <v>0</v>
+      <c r="C139" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>736</v>
@@ -9265,8 +9226,8 @@
       <c r="B140" s="2">
         <v>3</v>
       </c>
-      <c r="C140" s="2" t="b">
-        <v>0</v>
+      <c r="C140" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>737</v>
@@ -9279,8 +9240,8 @@
       <c r="B141" s="2">
         <v>4</v>
       </c>
-      <c r="C141" s="2" t="b">
-        <v>0</v>
+      <c r="C141" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>738</v>
@@ -9293,8 +9254,8 @@
       <c r="B142" s="2">
         <v>1</v>
       </c>
-      <c r="C142" s="2" t="b">
-        <v>0</v>
+      <c r="C142" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>739</v>
@@ -9307,8 +9268,8 @@
       <c r="B143" s="2">
         <v>2</v>
       </c>
-      <c r="C143" s="2" t="b">
-        <v>0</v>
+      <c r="C143" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>740</v>
@@ -9321,8 +9282,8 @@
       <c r="B144" s="2">
         <v>3</v>
       </c>
-      <c r="C144" s="2" t="b">
-        <v>0</v>
+      <c r="C144" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>741</v>
@@ -9335,8 +9296,8 @@
       <c r="B145" s="2">
         <v>1</v>
       </c>
-      <c r="C145" s="2" t="b">
-        <v>0</v>
+      <c r="C145" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>742</v>
@@ -9349,8 +9310,8 @@
       <c r="B146" s="2">
         <v>2</v>
       </c>
-      <c r="C146" s="2" t="b">
-        <v>0</v>
+      <c r="C146" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>743</v>
@@ -9363,8 +9324,8 @@
       <c r="B147" s="2">
         <v>3</v>
       </c>
-      <c r="C147" s="2" t="b">
-        <v>0</v>
+      <c r="C147" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>741</v>
@@ -9377,8 +9338,8 @@
       <c r="B148" s="2">
         <v>1</v>
       </c>
-      <c r="C148" s="2" t="b">
-        <v>0</v>
+      <c r="C148" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>739</v>
@@ -9391,8 +9352,8 @@
       <c r="B149" s="2">
         <v>2</v>
       </c>
-      <c r="C149" s="2" t="b">
-        <v>0</v>
+      <c r="C149" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>740</v>
@@ -9405,8 +9366,8 @@
       <c r="B150" s="2">
         <v>3</v>
       </c>
-      <c r="C150" s="2" t="b">
-        <v>0</v>
+      <c r="C150" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>741</v>
@@ -9419,8 +9380,8 @@
       <c r="B151" s="2">
         <v>1</v>
       </c>
-      <c r="C151" s="2" t="b">
-        <v>0</v>
+      <c r="C151" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>735</v>
@@ -9433,8 +9394,8 @@
       <c r="B152" s="2">
         <v>2</v>
       </c>
-      <c r="C152" s="2" t="b">
-        <v>0</v>
+      <c r="C152" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>736</v>
@@ -9447,8 +9408,8 @@
       <c r="B153" s="2">
         <v>3</v>
       </c>
-      <c r="C153" s="2" t="b">
-        <v>0</v>
+      <c r="C153" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>737</v>
@@ -9461,8 +9422,8 @@
       <c r="B154" s="2">
         <v>4</v>
       </c>
-      <c r="C154" s="2" t="b">
-        <v>0</v>
+      <c r="C154" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>738</v>
@@ -9475,8 +9436,8 @@
       <c r="B155" s="2">
         <v>0</v>
       </c>
-      <c r="C155" s="2" t="b">
-        <v>0</v>
+      <c r="C155" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>704</v>
@@ -9489,8 +9450,8 @@
       <c r="B156" s="2">
         <v>1</v>
       </c>
-      <c r="C156" s="2" t="b">
-        <v>0</v>
+      <c r="C156" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>705</v>
@@ -9503,8 +9464,8 @@
       <c r="B157" s="2">
         <v>1</v>
       </c>
-      <c r="C157" s="2" t="b">
-        <v>0</v>
+      <c r="C157" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>735</v>
@@ -9517,8 +9478,8 @@
       <c r="B158" s="2">
         <v>2</v>
       </c>
-      <c r="C158" s="2" t="b">
-        <v>0</v>
+      <c r="C158" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>736</v>
@@ -9531,8 +9492,8 @@
       <c r="B159" s="2">
         <v>3</v>
       </c>
-      <c r="C159" s="2" t="b">
-        <v>0</v>
+      <c r="C159" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>737</v>
@@ -9545,8 +9506,8 @@
       <c r="B160" s="2">
         <v>4</v>
       </c>
-      <c r="C160" s="2" t="b">
-        <v>0</v>
+      <c r="C160" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>738</v>
@@ -9559,8 +9520,8 @@
       <c r="B161" s="2">
         <v>0</v>
       </c>
-      <c r="C161" s="2" t="b">
-        <v>0</v>
+      <c r="C161" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>744</v>
@@ -9573,8 +9534,8 @@
       <c r="B162" s="2">
         <v>1</v>
       </c>
-      <c r="C162" s="2" t="b">
-        <v>0</v>
+      <c r="C162" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>745</v>
@@ -9587,8 +9548,8 @@
       <c r="B163" s="2">
         <v>2</v>
       </c>
-      <c r="C163" s="2" t="b">
-        <v>0</v>
+      <c r="C163" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>746</v>
@@ -9601,8 +9562,8 @@
       <c r="B164" s="2">
         <v>1</v>
       </c>
-      <c r="C164" s="2" t="b">
-        <v>0</v>
+      <c r="C164" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>735</v>
@@ -9615,8 +9576,8 @@
       <c r="B165" s="2">
         <v>2</v>
       </c>
-      <c r="C165" s="2" t="b">
-        <v>0</v>
+      <c r="C165" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>736</v>
@@ -9629,8 +9590,8 @@
       <c r="B166" s="2">
         <v>3</v>
       </c>
-      <c r="C166" s="2" t="b">
-        <v>0</v>
+      <c r="C166" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>737</v>
@@ -9643,8 +9604,8 @@
       <c r="B167" s="2">
         <v>4</v>
       </c>
-      <c r="C167" s="2" t="b">
-        <v>0</v>
+      <c r="C167" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>738</v>
@@ -9657,8 +9618,8 @@
       <c r="B168" s="2">
         <v>0</v>
       </c>
-      <c r="C168" s="2" t="b">
-        <v>0</v>
+      <c r="C168" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>744</v>
@@ -9671,8 +9632,8 @@
       <c r="B169" s="2">
         <v>1</v>
       </c>
-      <c r="C169" s="2" t="b">
-        <v>0</v>
+      <c r="C169" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>745</v>
@@ -9685,8 +9646,8 @@
       <c r="B170" s="2">
         <v>2</v>
       </c>
-      <c r="C170" s="2" t="b">
-        <v>0</v>
+      <c r="C170" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>746</v>
@@ -9699,8 +9660,8 @@
       <c r="B171" s="2">
         <v>1</v>
       </c>
-      <c r="C171" s="2" t="b">
-        <v>0</v>
+      <c r="C171" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>735</v>
@@ -9713,8 +9674,8 @@
       <c r="B172" s="2">
         <v>2</v>
       </c>
-      <c r="C172" s="2" t="b">
-        <v>0</v>
+      <c r="C172" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>736</v>
@@ -9727,8 +9688,8 @@
       <c r="B173" s="2">
         <v>3</v>
       </c>
-      <c r="C173" s="2" t="b">
-        <v>0</v>
+      <c r="C173" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>737</v>
@@ -9741,8 +9702,8 @@
       <c r="B174" s="2">
         <v>4</v>
       </c>
-      <c r="C174" s="2" t="b">
-        <v>0</v>
+      <c r="C174" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>738</v>
@@ -9755,8 +9716,8 @@
       <c r="B175" s="2">
         <v>1</v>
       </c>
-      <c r="C175" s="2" t="b">
-        <v>0</v>
+      <c r="C175" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>695</v>
@@ -9769,8 +9730,8 @@
       <c r="B176" s="2">
         <v>2</v>
       </c>
-      <c r="C176" s="2" t="b">
-        <v>0</v>
+      <c r="C176" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>747</v>
@@ -9783,8 +9744,8 @@
       <c r="B177" s="2">
         <v>3</v>
       </c>
-      <c r="C177" s="2" t="b">
-        <v>0</v>
+      <c r="C177" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>748</v>
@@ -9797,8 +9758,8 @@
       <c r="B178" s="2">
         <v>4</v>
       </c>
-      <c r="C178" s="2" t="b">
-        <v>0</v>
+      <c r="C178" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>703</v>
@@ -9811,8 +9772,8 @@
       <c r="B179" s="2">
         <v>0</v>
       </c>
-      <c r="C179" s="2" t="b">
-        <v>0</v>
+      <c r="C179" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>704</v>
@@ -9825,8 +9786,8 @@
       <c r="B180" s="2">
         <v>1</v>
       </c>
-      <c r="C180" s="2" t="b">
-        <v>0</v>
+      <c r="C180" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>705</v>
@@ -9839,8 +9800,8 @@
       <c r="B181" s="2">
         <v>0</v>
       </c>
-      <c r="C181" s="2" t="b">
-        <v>0</v>
+      <c r="C181" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>704</v>
@@ -9853,8 +9814,8 @@
       <c r="B182" s="2">
         <v>1</v>
       </c>
-      <c r="C182" s="2" t="b">
-        <v>0</v>
+      <c r="C182" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>705</v>
@@ -9867,8 +9828,8 @@
       <c r="B183" s="2">
         <v>0</v>
       </c>
-      <c r="C183" s="2" t="b">
-        <v>0</v>
+      <c r="C183" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>704</v>
@@ -9881,8 +9842,8 @@
       <c r="B184" s="2">
         <v>1</v>
       </c>
-      <c r="C184" s="2" t="b">
-        <v>0</v>
+      <c r="C184" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>705</v>
@@ -9895,8 +9856,8 @@
       <c r="B185" s="2">
         <v>0</v>
       </c>
-      <c r="C185" s="2" t="b">
-        <v>0</v>
+      <c r="C185" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>749</v>
@@ -9909,8 +9870,8 @@
       <c r="B186" s="2">
         <v>1</v>
       </c>
-      <c r="C186" s="2" t="b">
-        <v>0</v>
+      <c r="C186" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>750</v>
@@ -9923,8 +9884,8 @@
       <c r="B187" s="2">
         <v>2</v>
       </c>
-      <c r="C187" s="2" t="b">
-        <v>0</v>
+      <c r="C187" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>751</v>
@@ -9937,8 +9898,8 @@
       <c r="B188" s="2">
         <v>1</v>
       </c>
-      <c r="C188" s="2" t="b">
-        <v>0</v>
+      <c r="C188" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>735</v>
@@ -9951,8 +9912,8 @@
       <c r="B189" s="2">
         <v>2</v>
       </c>
-      <c r="C189" s="2" t="b">
-        <v>0</v>
+      <c r="C189" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>736</v>
@@ -9965,8 +9926,8 @@
       <c r="B190" s="2">
         <v>3</v>
       </c>
-      <c r="C190" s="2" t="b">
-        <v>0</v>
+      <c r="C190" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>737</v>
@@ -9979,8 +9940,8 @@
       <c r="B191" s="2">
         <v>4</v>
       </c>
-      <c r="C191" s="2" t="b">
-        <v>0</v>
+      <c r="C191" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>738</v>
@@ -9993,8 +9954,8 @@
       <c r="B192" s="2">
         <v>0</v>
       </c>
-      <c r="C192" s="2" t="b">
-        <v>0</v>
+      <c r="C192" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>704</v>
@@ -10007,8 +9968,8 @@
       <c r="B193" s="2">
         <v>1</v>
       </c>
-      <c r="C193" s="2" t="b">
-        <v>0</v>
+      <c r="C193" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>705</v>
@@ -10021,8 +9982,8 @@
       <c r="B194" s="2">
         <v>1</v>
       </c>
-      <c r="C194" s="2" t="b">
-        <v>0</v>
+      <c r="C194" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>752</v>
@@ -10035,8 +9996,8 @@
       <c r="B195" s="2">
         <v>2</v>
       </c>
-      <c r="C195" s="2" t="b">
-        <v>0</v>
+      <c r="C195" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>753</v>
@@ -10049,8 +10010,8 @@
       <c r="B196" s="2">
         <v>1</v>
       </c>
-      <c r="C196" s="2" t="b">
-        <v>0</v>
+      <c r="C196" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>754</v>
@@ -10063,8 +10024,8 @@
       <c r="B197" s="2">
         <v>2</v>
       </c>
-      <c r="C197" s="2" t="b">
-        <v>0</v>
+      <c r="C197" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>755</v>
@@ -10077,8 +10038,8 @@
       <c r="B198" s="2">
         <v>3</v>
       </c>
-      <c r="C198" s="2" t="b">
-        <v>0</v>
+      <c r="C198" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>756</v>
@@ -10091,8 +10052,8 @@
       <c r="B199" s="2">
         <v>1</v>
       </c>
-      <c r="C199" s="2" t="b">
-        <v>0</v>
+      <c r="C199" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>757</v>
@@ -10105,8 +10066,8 @@
       <c r="B200" s="2">
         <v>2</v>
       </c>
-      <c r="C200" s="2" t="b">
-        <v>0</v>
+      <c r="C200" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>758</v>
@@ -10119,8 +10080,8 @@
       <c r="B201" s="2">
         <v>3</v>
       </c>
-      <c r="C201" s="2" t="b">
-        <v>0</v>
+      <c r="C201" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>759</v>
@@ -10133,8 +10094,8 @@
       <c r="B202" s="2">
         <v>0</v>
       </c>
-      <c r="C202" s="2" t="b">
-        <v>0</v>
+      <c r="C202" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>704</v>
@@ -10147,8 +10108,8 @@
       <c r="B203" s="2">
         <v>1</v>
       </c>
-      <c r="C203" s="2" t="b">
-        <v>0</v>
+      <c r="C203" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>705</v>
@@ -10161,8 +10122,8 @@
       <c r="B204" s="2">
         <v>0</v>
       </c>
-      <c r="C204" s="2" t="b">
-        <v>0</v>
+      <c r="C204" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>704</v>
@@ -10175,8 +10136,8 @@
       <c r="B205" s="2">
         <v>1</v>
       </c>
-      <c r="C205" s="2" t="b">
-        <v>0</v>
+      <c r="C205" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>705</v>
@@ -10189,8 +10150,8 @@
       <c r="B206" s="2">
         <v>0</v>
       </c>
-      <c r="C206" s="2" t="b">
-        <v>0</v>
+      <c r="C206" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>704</v>
@@ -10203,8 +10164,8 @@
       <c r="B207" s="2">
         <v>1</v>
       </c>
-      <c r="C207" s="2" t="b">
-        <v>0</v>
+      <c r="C207" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>705</v>
@@ -10217,8 +10178,8 @@
       <c r="B208" s="2">
         <v>1</v>
       </c>
-      <c r="C208" s="2" t="b">
-        <v>0</v>
+      <c r="C208" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>718</v>
@@ -10231,8 +10192,8 @@
       <c r="B209" s="2">
         <v>2</v>
       </c>
-      <c r="C209" s="2" t="b">
-        <v>0</v>
+      <c r="C209" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>719</v>
@@ -10245,8 +10206,8 @@
       <c r="B210" s="2">
         <v>3</v>
       </c>
-      <c r="C210" s="2" t="b">
-        <v>0</v>
+      <c r="C210" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>720</v>
@@ -10259,8 +10220,8 @@
       <c r="B211" s="2">
         <v>4</v>
       </c>
-      <c r="C211" s="2" t="b">
-        <v>0</v>
+      <c r="C211" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>760</v>
@@ -10273,8 +10234,8 @@
       <c r="B212" s="2">
         <v>5</v>
       </c>
-      <c r="C212" s="2" t="b">
-        <v>0</v>
+      <c r="C212" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>761</v>
@@ -10287,8 +10248,8 @@
       <c r="B213" s="2">
         <v>0</v>
       </c>
-      <c r="C213" s="2" t="b">
-        <v>0</v>
+      <c r="C213" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>704</v>
@@ -10301,8 +10262,8 @@
       <c r="B214" s="2">
         <v>1</v>
       </c>
-      <c r="C214" s="2" t="b">
-        <v>0</v>
+      <c r="C214" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>705</v>
@@ -10315,8 +10276,8 @@
       <c r="B215" s="2">
         <v>0</v>
       </c>
-      <c r="C215" s="2" t="b">
-        <v>0</v>
+      <c r="C215" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>762</v>
@@ -10329,8 +10290,8 @@
       <c r="B216" s="2">
         <v>1</v>
       </c>
-      <c r="C216" s="2" t="b">
-        <v>0</v>
+      <c r="C216" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>763</v>
@@ -10343,8 +10304,8 @@
       <c r="B217" s="2">
         <v>1</v>
       </c>
-      <c r="C217" s="2" t="b">
-        <v>0</v>
+      <c r="C217" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>764</v>
@@ -10357,8 +10318,8 @@
       <c r="B218" s="2">
         <v>2</v>
       </c>
-      <c r="C218" s="2" t="b">
-        <v>0</v>
+      <c r="C218" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>765</v>
@@ -10371,8 +10332,8 @@
       <c r="B219" s="2">
         <v>3</v>
       </c>
-      <c r="C219" s="2" t="b">
-        <v>0</v>
+      <c r="C219" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>766</v>
@@ -10385,8 +10346,8 @@
       <c r="B220" s="2">
         <v>4</v>
       </c>
-      <c r="C220" s="2" t="b">
-        <v>0</v>
+      <c r="C220" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>767</v>
@@ -10399,8 +10360,8 @@
       <c r="B221" s="2">
         <v>5</v>
       </c>
-      <c r="C221" s="2" t="b">
-        <v>0</v>
+      <c r="C221" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>768</v>
@@ -10413,8 +10374,8 @@
       <c r="B222" s="2">
         <v>1</v>
       </c>
-      <c r="C222" s="2" t="b">
-        <v>0</v>
+      <c r="C222" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>769</v>
@@ -10427,8 +10388,8 @@
       <c r="B223" s="2">
         <v>2</v>
       </c>
-      <c r="C223" s="2" t="b">
-        <v>0</v>
+      <c r="C223" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>770</v>
@@ -10441,8 +10402,8 @@
       <c r="B224" s="2">
         <v>3</v>
       </c>
-      <c r="C224" s="2" t="b">
-        <v>0</v>
+      <c r="C224" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>771</v>
@@ -10455,8 +10416,8 @@
       <c r="B225" s="2">
         <v>4</v>
       </c>
-      <c r="C225" s="2" t="b">
-        <v>0</v>
+      <c r="C225" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>772</v>
@@ -10469,8 +10430,8 @@
       <c r="B226" s="2">
         <v>5</v>
       </c>
-      <c r="C226" s="2" t="b">
-        <v>0</v>
+      <c r="C226" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>773</v>
@@ -10483,8 +10444,8 @@
       <c r="B227" s="2">
         <v>0</v>
       </c>
-      <c r="C227" s="2" t="b">
-        <v>0</v>
+      <c r="C227" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>774</v>
@@ -10497,8 +10458,8 @@
       <c r="B228" s="2">
         <v>1</v>
       </c>
-      <c r="C228" s="2" t="b">
-        <v>0</v>
+      <c r="C228" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>775</v>
@@ -10511,8 +10472,8 @@
       <c r="B229" s="2">
         <v>2</v>
       </c>
-      <c r="C229" s="2" t="b">
-        <v>0</v>
+      <c r="C229" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>776</v>
@@ -10525,8 +10486,8 @@
       <c r="B230" s="2">
         <v>3</v>
       </c>
-      <c r="C230" s="2" t="b">
-        <v>0</v>
+      <c r="C230" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>777</v>
@@ -10539,8 +10500,8 @@
       <c r="B231" s="2">
         <v>4</v>
       </c>
-      <c r="C231" s="2" t="b">
-        <v>0</v>
+      <c r="C231" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>778</v>
@@ -10553,8 +10514,8 @@
       <c r="B232" s="2">
         <v>5</v>
       </c>
-      <c r="C232" s="2" t="b">
-        <v>0</v>
+      <c r="C232" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>779</v>
@@ -10567,8 +10528,8 @@
       <c r="B233" s="2">
         <v>6</v>
       </c>
-      <c r="C233" s="2" t="b">
-        <v>0</v>
+      <c r="C233" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>780</v>
@@ -10581,8 +10542,8 @@
       <c r="B234" s="2">
         <v>7</v>
       </c>
-      <c r="C234" s="2" t="b">
-        <v>0</v>
+      <c r="C234" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>781</v>
@@ -10595,8 +10556,8 @@
       <c r="B235" s="2">
         <v>8</v>
       </c>
-      <c r="C235" s="2" t="b">
-        <v>0</v>
+      <c r="C235" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>782</v>
@@ -10609,8 +10570,8 @@
       <c r="B236" s="2">
         <v>9</v>
       </c>
-      <c r="C236" s="2" t="b">
-        <v>0</v>
+      <c r="C236" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>783</v>
@@ -10623,8 +10584,8 @@
       <c r="B237" s="2">
         <v>0</v>
       </c>
-      <c r="C237" s="2" t="b">
-        <v>0</v>
+      <c r="C237" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>774</v>
@@ -10637,8 +10598,8 @@
       <c r="B238" s="2">
         <v>1</v>
       </c>
-      <c r="C238" s="2" t="b">
-        <v>0</v>
+      <c r="C238" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>775</v>
@@ -10651,8 +10612,8 @@
       <c r="B239" s="2">
         <v>2</v>
       </c>
-      <c r="C239" s="2" t="b">
-        <v>0</v>
+      <c r="C239" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>776</v>
@@ -10665,8 +10626,8 @@
       <c r="B240" s="2">
         <v>3</v>
       </c>
-      <c r="C240" s="2" t="b">
-        <v>0</v>
+      <c r="C240" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>777</v>
@@ -10679,8 +10640,8 @@
       <c r="B241" s="2">
         <v>4</v>
       </c>
-      <c r="C241" s="2" t="b">
-        <v>0</v>
+      <c r="C241" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>778</v>
@@ -10693,8 +10654,8 @@
       <c r="B242" s="2">
         <v>5</v>
       </c>
-      <c r="C242" s="2" t="b">
-        <v>0</v>
+      <c r="C242" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>779</v>
@@ -10707,8 +10668,8 @@
       <c r="B243" s="2">
         <v>6</v>
       </c>
-      <c r="C243" s="2" t="b">
-        <v>0</v>
+      <c r="C243" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>780</v>
@@ -10721,8 +10682,8 @@
       <c r="B244" s="2">
         <v>7</v>
       </c>
-      <c r="C244" s="2" t="b">
-        <v>0</v>
+      <c r="C244" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>781</v>
@@ -10735,8 +10696,8 @@
       <c r="B245" s="2">
         <v>8</v>
       </c>
-      <c r="C245" s="2" t="b">
-        <v>0</v>
+      <c r="C245" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>782</v>
@@ -10749,8 +10710,8 @@
       <c r="B246" s="2">
         <v>9</v>
       </c>
-      <c r="C246" s="2" t="b">
-        <v>0</v>
+      <c r="C246" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>783</v>
@@ -10763,8 +10724,8 @@
       <c r="B247" s="2">
         <v>1001</v>
       </c>
-      <c r="C247" s="2" t="b">
-        <v>0</v>
+      <c r="C247" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>784</v>
@@ -10777,8 +10738,8 @@
       <c r="B248" s="2">
         <v>1102</v>
       </c>
-      <c r="C248" s="2" t="b">
-        <v>0</v>
+      <c r="C248" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>785</v>
@@ -10791,8 +10752,8 @@
       <c r="B249" s="2">
         <v>1103</v>
       </c>
-      <c r="C249" s="2" t="b">
-        <v>0</v>
+      <c r="C249" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>786</v>
@@ -10805,8 +10766,8 @@
       <c r="B250" s="2">
         <v>1104</v>
       </c>
-      <c r="C250" s="2" t="b">
-        <v>0</v>
+      <c r="C250" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>787</v>
@@ -10819,8 +10780,8 @@
       <c r="B251" s="2">
         <v>1201</v>
       </c>
-      <c r="C251" s="2" t="b">
-        <v>0</v>
+      <c r="C251" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>788</v>
@@ -10833,8 +10794,8 @@
       <c r="B252" s="2">
         <v>1202</v>
       </c>
-      <c r="C252" s="2" t="b">
-        <v>0</v>
+      <c r="C252" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>789</v>
@@ -10847,8 +10808,8 @@
       <c r="B253" s="2">
         <v>1203</v>
       </c>
-      <c r="C253" s="2" t="b">
-        <v>0</v>
+      <c r="C253" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>790</v>
@@ -10861,8 +10822,8 @@
       <c r="B254" s="2">
         <v>1301</v>
       </c>
-      <c r="C254" s="2" t="b">
-        <v>0</v>
+      <c r="C254" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>791</v>
@@ -10875,8 +10836,8 @@
       <c r="B255" s="2">
         <v>1401</v>
       </c>
-      <c r="C255" s="2" t="b">
-        <v>0</v>
+      <c r="C255" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>792</v>
@@ -10889,8 +10850,8 @@
       <c r="B256" s="2">
         <v>1501</v>
       </c>
-      <c r="C256" s="2" t="b">
-        <v>0</v>
+      <c r="C256" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>793</v>
@@ -10903,8 +10864,8 @@
       <c r="B257" s="2">
         <v>1601</v>
       </c>
-      <c r="C257" s="2" t="b">
-        <v>0</v>
+      <c r="C257" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>794</v>
@@ -10917,8 +10878,8 @@
       <c r="B258" s="2">
         <v>1701</v>
       </c>
-      <c r="C258" s="2" t="b">
-        <v>0</v>
+      <c r="C258" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D258" s="2" t="s">
         <v>795</v>
@@ -10931,8 +10892,8 @@
       <c r="B259" s="2">
         <v>1801</v>
       </c>
-      <c r="C259" s="2" t="b">
-        <v>0</v>
+      <c r="C259" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>796</v>
@@ -10945,8 +10906,8 @@
       <c r="B260" s="2">
         <v>1802</v>
       </c>
-      <c r="C260" s="2" t="b">
-        <v>0</v>
+      <c r="C260" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>797</v>
@@ -10959,8 +10920,8 @@
       <c r="B261" s="2">
         <v>1901</v>
       </c>
-      <c r="C261" s="2" t="b">
-        <v>0</v>
+      <c r="C261" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>798</v>
@@ -10973,8 +10934,8 @@
       <c r="B262" s="2">
         <v>2001</v>
       </c>
-      <c r="C262" s="2" t="b">
-        <v>0</v>
+      <c r="C262" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>799</v>
@@ -10987,8 +10948,8 @@
       <c r="B263" s="2">
         <v>1</v>
       </c>
-      <c r="C263" s="2" t="b">
-        <v>0</v>
+      <c r="C263" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>705</v>
@@ -11001,8 +10962,8 @@
       <c r="B264" s="2">
         <v>0</v>
       </c>
-      <c r="C264" s="2" t="b">
-        <v>0</v>
+      <c r="C264" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>704</v>
@@ -11015,8 +10976,8 @@
       <c r="B265" s="2">
         <v>1</v>
       </c>
-      <c r="C265" s="2" t="b">
-        <v>0</v>
+      <c r="C265" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>705</v>
@@ -11029,8 +10990,8 @@
       <c r="B266" s="2">
         <v>0</v>
       </c>
-      <c r="C266" s="2" t="b">
-        <v>0</v>
+      <c r="C266" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>704</v>
@@ -11043,8 +11004,8 @@
       <c r="B267" s="2">
         <v>1</v>
       </c>
-      <c r="C267" s="2" t="b">
-        <v>0</v>
+      <c r="C267" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>800</v>
@@ -11057,8 +11018,8 @@
       <c r="B268" s="2">
         <v>2</v>
       </c>
-      <c r="C268" s="2" t="b">
-        <v>0</v>
+      <c r="C268" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D268" s="2" t="s">
         <v>801</v>
@@ -11071,8 +11032,8 @@
       <c r="B269" s="2">
         <v>3</v>
       </c>
-      <c r="C269" s="2" t="b">
-        <v>0</v>
+      <c r="C269" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>802</v>
@@ -11085,8 +11046,8 @@
       <c r="B270" s="2">
         <v>4</v>
       </c>
-      <c r="C270" s="2" t="b">
-        <v>0</v>
+      <c r="C270" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>803</v>
@@ -11099,8 +11060,8 @@
       <c r="B271" s="2">
         <v>5</v>
       </c>
-      <c r="C271" s="2" t="b">
-        <v>0</v>
+      <c r="C271" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>804</v>
@@ -11113,8 +11074,8 @@
       <c r="B272" s="2">
         <v>6</v>
       </c>
-      <c r="C272" s="2" t="b">
-        <v>0</v>
+      <c r="C272" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>805</v>
@@ -11127,8 +11088,8 @@
       <c r="B273" s="2">
         <v>1</v>
       </c>
-      <c r="C273" s="2" t="b">
-        <v>0</v>
+      <c r="C273" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D273" s="2" t="s">
         <v>806</v>
@@ -11141,8 +11102,8 @@
       <c r="B274" s="2">
         <v>2</v>
       </c>
-      <c r="C274" s="2" t="b">
-        <v>0</v>
+      <c r="C274" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D274" s="2" t="s">
         <v>802</v>
@@ -11155,8 +11116,8 @@
       <c r="B275" s="2">
         <v>3</v>
       </c>
-      <c r="C275" s="2" t="b">
-        <v>0</v>
+      <c r="C275" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>803</v>
@@ -11169,8 +11130,8 @@
       <c r="B276" s="2">
         <v>4</v>
       </c>
-      <c r="C276" s="2" t="b">
-        <v>0</v>
+      <c r="C276" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>804</v>
@@ -11183,8 +11144,8 @@
       <c r="B277" s="2">
         <v>5</v>
       </c>
-      <c r="C277" s="2" t="b">
-        <v>0</v>
+      <c r="C277" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>807</v>
@@ -11197,8 +11158,8 @@
       <c r="B278" s="2">
         <v>6</v>
       </c>
-      <c r="C278" s="2" t="b">
-        <v>0</v>
+      <c r="C278" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D278" s="2" t="s">
         <v>808</v>
@@ -11211,8 +11172,8 @@
       <c r="B279" s="2">
         <v>1</v>
       </c>
-      <c r="C279" s="2" t="b">
-        <v>0</v>
+      <c r="C279" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>809</v>
@@ -11225,8 +11186,8 @@
       <c r="B280" s="2">
         <v>2</v>
       </c>
-      <c r="C280" s="2" t="b">
-        <v>0</v>
+      <c r="C280" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>810</v>
@@ -11239,8 +11200,8 @@
       <c r="B281" s="2">
         <v>3</v>
       </c>
-      <c r="C281" s="2" t="b">
-        <v>0</v>
+      <c r="C281" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>811</v>
@@ -11253,8 +11214,8 @@
       <c r="B282" s="2">
         <v>1</v>
       </c>
-      <c r="C282" s="2" t="b">
-        <v>0</v>
+      <c r="C282" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>809</v>
@@ -11267,8 +11228,8 @@
       <c r="B283" s="2">
         <v>2</v>
       </c>
-      <c r="C283" s="2" t="b">
-        <v>0</v>
+      <c r="C283" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>812</v>
@@ -11281,8 +11242,8 @@
       <c r="B284" s="2">
         <v>3</v>
       </c>
-      <c r="C284" s="2" t="b">
-        <v>0</v>
+      <c r="C284" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>810</v>
@@ -11295,8 +11256,8 @@
       <c r="B285" s="2">
         <v>4</v>
       </c>
-      <c r="C285" s="2" t="b">
-        <v>0</v>
+      <c r="C285" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>813</v>
@@ -11309,8 +11270,8 @@
       <c r="B286" s="2">
         <v>5</v>
       </c>
-      <c r="C286" s="2" t="b">
-        <v>0</v>
+      <c r="C286" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>811</v>
@@ -11323,8 +11284,8 @@
       <c r="B287" s="2">
         <v>1</v>
       </c>
-      <c r="C287" s="2" t="b">
-        <v>0</v>
+      <c r="C287" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>814</v>
@@ -11337,8 +11298,8 @@
       <c r="B288" s="2">
         <v>2</v>
       </c>
-      <c r="C288" s="2" t="b">
-        <v>0</v>
+      <c r="C288" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>815</v>
@@ -11351,8 +11312,8 @@
       <c r="B289" s="2">
         <v>3</v>
       </c>
-      <c r="C289" s="2" t="b">
-        <v>0</v>
+      <c r="C289" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>816</v>
@@ -11365,8 +11326,8 @@
       <c r="B290" s="2">
         <v>1</v>
       </c>
-      <c r="C290" s="2" t="b">
-        <v>0</v>
+      <c r="C290" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>814</v>
@@ -11379,8 +11340,8 @@
       <c r="B291" s="2">
         <v>2</v>
       </c>
-      <c r="C291" s="2" t="b">
-        <v>0</v>
+      <c r="C291" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>815</v>
@@ -11393,8 +11354,8 @@
       <c r="B292" s="2">
         <v>3</v>
       </c>
-      <c r="C292" s="2" t="b">
-        <v>0</v>
+      <c r="C292" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>816</v>
@@ -11407,8 +11368,8 @@
       <c r="B293" s="2">
         <v>1</v>
       </c>
-      <c r="C293" s="2" t="b">
-        <v>0</v>
+      <c r="C293" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>814</v>
@@ -11421,8 +11382,8 @@
       <c r="B294" s="2">
         <v>2</v>
       </c>
-      <c r="C294" s="2" t="b">
-        <v>0</v>
+      <c r="C294" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>815</v>
@@ -11435,8 +11396,8 @@
       <c r="B295" s="2">
         <v>3</v>
       </c>
-      <c r="C295" s="2" t="b">
-        <v>0</v>
+      <c r="C295" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>816</v>
@@ -11449,8 +11410,8 @@
       <c r="B296" s="2">
         <v>0</v>
       </c>
-      <c r="C296" s="2" t="b">
-        <v>0</v>
+      <c r="C296" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>695</v>
@@ -11463,8 +11424,8 @@
       <c r="B297" s="2">
         <v>1</v>
       </c>
-      <c r="C297" s="2" t="b">
-        <v>0</v>
+      <c r="C297" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>696</v>
@@ -11477,8 +11438,8 @@
       <c r="B298" s="2">
         <v>0</v>
       </c>
-      <c r="C298" s="2" t="b">
-        <v>0</v>
+      <c r="C298" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>695</v>
@@ -11491,8 +11452,8 @@
       <c r="B299" s="2">
         <v>1</v>
       </c>
-      <c r="C299" s="2" t="b">
-        <v>0</v>
+      <c r="C299" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>696</v>
@@ -11505,8 +11466,8 @@
       <c r="B300" s="2">
         <v>0</v>
       </c>
-      <c r="C300" s="2" t="b">
-        <v>0</v>
+      <c r="C300" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>695</v>
@@ -11519,8 +11480,8 @@
       <c r="B301" s="2">
         <v>1</v>
       </c>
-      <c r="C301" s="2" t="b">
-        <v>0</v>
+      <c r="C301" s="2" t="s">
+        <v>817</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>696</v>

</xml_diff>

<commit_message>
converted text true/false to boolean value
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474B4FF0-F4F7-4746-836B-5022AC0F1699}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="16164" windowHeight="10236" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2156" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="817">
   <si>
     <t>name</t>
   </si>
@@ -2466,15 +2472,12 @@
   </si>
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -2549,8 +2552,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2566,7 +2569,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2608,7 +2611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2640,9 +2643,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2674,6 +2695,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2849,20 +2888,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D313"/>
   <sheetViews>
     <sheetView topLeftCell="A283" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="197.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="1"/>
+    <col min="4" max="4" width="197.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -7256,21 +7295,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A282" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C301"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -7294,8 +7333,8 @@
       <c r="B2" s="2">
         <v>101</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>817</v>
+      <c r="C2" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>654</v>
@@ -7308,8 +7347,8 @@
       <c r="B3" s="2">
         <v>102</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>817</v>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>655</v>
@@ -7322,8 +7361,8 @@
       <c r="B4" s="2">
         <v>103</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>817</v>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>656</v>
@@ -7336,8 +7375,8 @@
       <c r="B5" s="2">
         <v>104</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>817</v>
+      <c r="C5" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>657</v>
@@ -7350,8 +7389,8 @@
       <c r="B6" s="2">
         <v>105</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>817</v>
+      <c r="C6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>658</v>
@@ -7364,8 +7403,8 @@
       <c r="B7" s="2">
         <v>106</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>817</v>
+      <c r="C7" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>659</v>
@@ -7378,8 +7417,8 @@
       <c r="B8" s="2">
         <v>107</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>817</v>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>660</v>
@@ -7392,8 +7431,8 @@
       <c r="B9" s="2">
         <v>108</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>817</v>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>661</v>
@@ -7406,8 +7445,8 @@
       <c r="B10" s="2">
         <v>109</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>817</v>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>662</v>
@@ -7420,8 +7459,8 @@
       <c r="B11" s="2">
         <v>110</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>817</v>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>663</v>
@@ -7434,8 +7473,8 @@
       <c r="B12" s="2">
         <v>111</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>817</v>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>664</v>
@@ -7448,8 +7487,8 @@
       <c r="B13" s="2">
         <v>112</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>817</v>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>665</v>
@@ -7462,8 +7501,8 @@
       <c r="B14" s="2">
         <v>113</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>817</v>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>666</v>
@@ -7476,8 +7515,8 @@
       <c r="B15" s="2">
         <v>114</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>817</v>
+      <c r="C15" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>667</v>
@@ -7490,8 +7529,8 @@
       <c r="B16" s="2">
         <v>115</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>817</v>
+      <c r="C16" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>668</v>
@@ -7504,8 +7543,8 @@
       <c r="B17" s="2">
         <v>116</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>817</v>
+      <c r="C17" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>669</v>
@@ -7518,8 +7557,8 @@
       <c r="B18" s="2">
         <v>117</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>817</v>
+      <c r="C18" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>670</v>
@@ -7532,8 +7571,8 @@
       <c r="B19" s="2">
         <v>118</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>817</v>
+      <c r="C19" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>671</v>
@@ -7546,8 +7585,8 @@
       <c r="B20" s="2">
         <v>119</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>817</v>
+      <c r="C20" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>672</v>
@@ -7560,8 +7599,8 @@
       <c r="B21" s="2">
         <v>120</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>817</v>
+      <c r="C21" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>673</v>
@@ -7574,8 +7613,8 @@
       <c r="B22" s="2">
         <v>121</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>817</v>
+      <c r="C22" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>674</v>
@@ -7588,8 +7627,8 @@
       <c r="B23" s="2">
         <v>122</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>817</v>
+      <c r="C23" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>675</v>
@@ -7602,8 +7641,8 @@
       <c r="B24" s="2">
         <v>36</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>817</v>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>676</v>
@@ -7616,8 +7655,8 @@
       <c r="B25" s="2">
         <v>208</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>817</v>
+      <c r="C25" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>677</v>
@@ -7630,8 +7669,8 @@
       <c r="B26" s="2">
         <v>246</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>817</v>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>678</v>
@@ -7644,8 +7683,8 @@
       <c r="B27" s="2">
         <v>250</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>817</v>
+      <c r="C27" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>679</v>
@@ -7658,8 +7697,8 @@
       <c r="B28" s="2">
         <v>276</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>817</v>
+      <c r="C28" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>680</v>
@@ -7672,8 +7711,8 @@
       <c r="B29" s="2">
         <v>300</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>817</v>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>681</v>
@@ -7686,8 +7725,8 @@
       <c r="B30" s="2">
         <v>380</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>817</v>
+      <c r="C30" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>682</v>
@@ -7700,8 +7739,8 @@
       <c r="B31" s="2">
         <v>528</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>817</v>
+      <c r="C31" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>683</v>
@@ -7714,8 +7753,8 @@
       <c r="B32" s="2">
         <v>578</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>817</v>
+      <c r="C32" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>684</v>
@@ -7728,8 +7767,8 @@
       <c r="B33" s="2">
         <v>724</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>817</v>
+      <c r="C33" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>685</v>
@@ -7742,8 +7781,8 @@
       <c r="B34" s="2">
         <v>826</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>817</v>
+      <c r="C34" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>686</v>
@@ -7756,8 +7795,8 @@
       <c r="B35" s="2">
         <v>0</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>817</v>
+      <c r="C35" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>687</v>
@@ -7770,8 +7809,8 @@
       <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>817</v>
+      <c r="C36" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>688</v>
@@ -7784,8 +7823,8 @@
       <c r="B37" s="2">
         <v>2</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>817</v>
+      <c r="C37" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>689</v>
@@ -7798,8 +7837,8 @@
       <c r="B38" s="2">
         <v>1</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>817</v>
+      <c r="C38" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>690</v>
@@ -7812,8 +7851,8 @@
       <c r="B39" s="2">
         <v>2</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>817</v>
+      <c r="C39" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>691</v>
@@ -7826,8 +7865,8 @@
       <c r="B40" s="2">
         <v>3</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>817</v>
+      <c r="C40" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>692</v>
@@ -7840,8 +7879,8 @@
       <c r="B41" s="2">
         <v>1</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>817</v>
+      <c r="C41" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>693</v>
@@ -7854,8 +7893,8 @@
       <c r="B42" s="2">
         <v>2</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>817</v>
+      <c r="C42" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>694</v>
@@ -7868,8 +7907,8 @@
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>817</v>
+      <c r="C43" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>692</v>
@@ -7882,8 +7921,8 @@
       <c r="B44" s="2">
         <v>1</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>817</v>
+      <c r="C44" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>690</v>
@@ -7896,8 +7935,8 @@
       <c r="B45" s="2">
         <v>2</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>817</v>
+      <c r="C45" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>691</v>
@@ -7910,8 +7949,8 @@
       <c r="B46" s="2">
         <v>3</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>817</v>
+      <c r="C46" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>692</v>
@@ -7924,8 +7963,8 @@
       <c r="B47" s="2">
         <v>0</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>817</v>
+      <c r="C47" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>695</v>
@@ -7938,8 +7977,8 @@
       <c r="B48" s="2">
         <v>1</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>817</v>
+      <c r="C48" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>696</v>
@@ -7952,8 +7991,8 @@
       <c r="B49" s="2">
         <v>0</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>817</v>
+      <c r="C49" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>697</v>
@@ -7966,8 +8005,8 @@
       <c r="B50" s="2">
         <v>1</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>817</v>
+      <c r="C50" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>698</v>
@@ -7980,8 +8019,8 @@
       <c r="B51" s="2">
         <v>0</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>817</v>
+      <c r="C51" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>697</v>
@@ -7994,8 +8033,8 @@
       <c r="B52" s="2">
         <v>1</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>817</v>
+      <c r="C52" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>698</v>
@@ -8008,8 +8047,8 @@
       <c r="B53" s="2">
         <v>0</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>817</v>
+      <c r="C53" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>697</v>
@@ -8022,8 +8061,8 @@
       <c r="B54" s="2">
         <v>1</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>817</v>
+      <c r="C54" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>698</v>
@@ -8036,8 +8075,8 @@
       <c r="B55" s="2">
         <v>2</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>817</v>
+      <c r="C55" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>699</v>
@@ -8050,8 +8089,8 @@
       <c r="B56" s="2">
         <v>3</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>817</v>
+      <c r="C56" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>700</v>
@@ -8064,8 +8103,8 @@
       <c r="B57" s="2">
         <v>0</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>817</v>
+      <c r="C57" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>697</v>
@@ -8078,8 +8117,8 @@
       <c r="B58" s="2">
         <v>1</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>817</v>
+      <c r="C58" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>698</v>
@@ -8092,8 +8131,8 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>817</v>
+      <c r="C59" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>695</v>
@@ -8106,8 +8145,8 @@
       <c r="B60" s="2">
         <v>2</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>817</v>
+      <c r="C60" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>701</v>
@@ -8120,8 +8159,8 @@
       <c r="B61" s="2">
         <v>3</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>817</v>
+      <c r="C61" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>702</v>
@@ -8134,8 +8173,8 @@
       <c r="B62" s="2">
         <v>4</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>817</v>
+      <c r="C62" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>380</v>
@@ -8148,8 +8187,8 @@
       <c r="B63" s="2">
         <v>5</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>817</v>
+      <c r="C63" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>703</v>
@@ -8162,8 +8201,8 @@
       <c r="B64" s="2">
         <v>0</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>817</v>
+      <c r="C64" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>704</v>
@@ -8176,8 +8215,8 @@
       <c r="B65" s="2">
         <v>1</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>817</v>
+      <c r="C65" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>705</v>
@@ -8190,8 +8229,8 @@
       <c r="B66" s="2">
         <v>0</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>817</v>
+      <c r="C66" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>704</v>
@@ -8204,8 +8243,8 @@
       <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>817</v>
+      <c r="C67" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>705</v>
@@ -8218,8 +8257,8 @@
       <c r="B68" s="2">
         <v>0</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>817</v>
+      <c r="C68" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>704</v>
@@ -8232,8 +8271,8 @@
       <c r="B69" s="2">
         <v>1</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>817</v>
+      <c r="C69" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>705</v>
@@ -8246,8 +8285,8 @@
       <c r="B70" s="2">
         <v>0</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>817</v>
+      <c r="C70" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>704</v>
@@ -8260,8 +8299,8 @@
       <c r="B71" s="2">
         <v>1</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>817</v>
+      <c r="C71" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>705</v>
@@ -8274,8 +8313,8 @@
       <c r="B72" s="2">
         <v>0</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>817</v>
+      <c r="C72" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>704</v>
@@ -8288,8 +8327,8 @@
       <c r="B73" s="2">
         <v>1</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>817</v>
+      <c r="C73" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>705</v>
@@ -8302,8 +8341,8 @@
       <c r="B74" s="2">
         <v>0</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>817</v>
+      <c r="C74" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>704</v>
@@ -8316,8 +8355,8 @@
       <c r="B75" s="2">
         <v>1</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>817</v>
+      <c r="C75" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>705</v>
@@ -8330,8 +8369,8 @@
       <c r="B76" s="2">
         <v>0</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>817</v>
+      <c r="C76" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>704</v>
@@ -8344,8 +8383,8 @@
       <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>817</v>
+      <c r="C77" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>705</v>
@@ -8358,8 +8397,8 @@
       <c r="B78" s="2">
         <v>0</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>817</v>
+      <c r="C78" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>704</v>
@@ -8372,8 +8411,8 @@
       <c r="B79" s="2">
         <v>1</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>817</v>
+      <c r="C79" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>705</v>
@@ -8386,8 +8425,8 @@
       <c r="B80" s="2">
         <v>0</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>817</v>
+      <c r="C80" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>704</v>
@@ -8400,8 +8439,8 @@
       <c r="B81" s="2">
         <v>1</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>817</v>
+      <c r="C81" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>705</v>
@@ -8414,8 +8453,8 @@
       <c r="B82" s="2">
         <v>0</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>817</v>
+      <c r="C82" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>704</v>
@@ -8428,8 +8467,8 @@
       <c r="B83" s="2">
         <v>1</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>817</v>
+      <c r="C83" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>705</v>
@@ -8442,8 +8481,8 @@
       <c r="B84" s="2">
         <v>0</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>817</v>
+      <c r="C84" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>706</v>
@@ -8456,8 +8495,8 @@
       <c r="B85" s="2">
         <v>1</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>817</v>
+      <c r="C85" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>707</v>
@@ -8470,8 +8509,8 @@
       <c r="B86" s="2">
         <v>2</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>817</v>
+      <c r="C86" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>708</v>
@@ -8484,8 +8523,8 @@
       <c r="B87" s="2">
         <v>0</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>817</v>
+      <c r="C87" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>704</v>
@@ -8498,8 +8537,8 @@
       <c r="B88" s="2">
         <v>1</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>817</v>
+      <c r="C88" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>705</v>
@@ -8512,8 +8551,8 @@
       <c r="B89" s="2">
         <v>0</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>817</v>
+      <c r="C89" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>706</v>
@@ -8526,8 +8565,8 @@
       <c r="B90" s="2">
         <v>1</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>817</v>
+      <c r="C90" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>707</v>
@@ -8540,8 +8579,8 @@
       <c r="B91" s="2">
         <v>2</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>817</v>
+      <c r="C91" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>708</v>
@@ -8554,8 +8593,8 @@
       <c r="B92" s="2">
         <v>0</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>817</v>
+      <c r="C92" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>704</v>
@@ -8568,8 +8607,8 @@
       <c r="B93" s="2">
         <v>1</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>817</v>
+      <c r="C93" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>705</v>
@@ -8582,8 +8621,8 @@
       <c r="B94" s="2">
         <v>0</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>817</v>
+      <c r="C94" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>709</v>
@@ -8596,8 +8635,8 @@
       <c r="B95" s="2">
         <v>1</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>817</v>
+      <c r="C95" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>710</v>
@@ -8610,8 +8649,8 @@
       <c r="B96" s="2">
         <v>2</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>817</v>
+      <c r="C96" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>711</v>
@@ -8624,8 +8663,8 @@
       <c r="B97" s="2">
         <v>3</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>817</v>
+      <c r="C97" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>712</v>
@@ -8638,8 +8677,8 @@
       <c r="B98" s="2">
         <v>4</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>817</v>
+      <c r="C98" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>713</v>
@@ -8652,8 +8691,8 @@
       <c r="B99" s="2">
         <v>0</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>817</v>
+      <c r="C99" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>704</v>
@@ -8666,8 +8705,8 @@
       <c r="B100" s="2">
         <v>1</v>
       </c>
-      <c r="C100" s="2" t="s">
-        <v>817</v>
+      <c r="C100" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>705</v>
@@ -8680,8 +8719,8 @@
       <c r="B101" s="2">
         <v>0</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>817</v>
+      <c r="C101" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>706</v>
@@ -8694,8 +8733,8 @@
       <c r="B102" s="2">
         <v>1</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>817</v>
+      <c r="C102" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>714</v>
@@ -8708,8 +8747,8 @@
       <c r="B103" s="2">
         <v>2</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>817</v>
+      <c r="C103" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>715</v>
@@ -8722,8 +8761,8 @@
       <c r="B104" s="2">
         <v>3</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>817</v>
+      <c r="C104" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>716</v>
@@ -8736,8 +8775,8 @@
       <c r="B105" s="2">
         <v>0</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>817</v>
+      <c r="C105" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>704</v>
@@ -8750,8 +8789,8 @@
       <c r="B106" s="2">
         <v>1</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>817</v>
+      <c r="C106" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>705</v>
@@ -8764,8 +8803,8 @@
       <c r="B107" s="2">
         <v>0</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>817</v>
+      <c r="C107" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>704</v>
@@ -8778,8 +8817,8 @@
       <c r="B108" s="2">
         <v>1</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>817</v>
+      <c r="C108" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>705</v>
@@ -8792,8 +8831,8 @@
       <c r="B109" s="2">
         <v>0</v>
       </c>
-      <c r="C109" s="2" t="s">
-        <v>817</v>
+      <c r="C109" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>704</v>
@@ -8806,8 +8845,8 @@
       <c r="B110" s="2">
         <v>1</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>817</v>
+      <c r="C110" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>705</v>
@@ -8820,8 +8859,8 @@
       <c r="B111" s="2">
         <v>0</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>817</v>
+      <c r="C111" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>717</v>
@@ -8834,8 +8873,8 @@
       <c r="B112" s="2">
         <v>1</v>
       </c>
-      <c r="C112" s="2" t="s">
-        <v>817</v>
+      <c r="C112" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>718</v>
@@ -8848,8 +8887,8 @@
       <c r="B113" s="2">
         <v>2</v>
       </c>
-      <c r="C113" s="2" t="s">
-        <v>817</v>
+      <c r="C113" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>719</v>
@@ -8862,8 +8901,8 @@
       <c r="B114" s="2">
         <v>3</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>817</v>
+      <c r="C114" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>720</v>
@@ -8876,8 +8915,8 @@
       <c r="B115" s="2">
         <v>4</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>817</v>
+      <c r="C115" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>721</v>
@@ -8890,8 +8929,8 @@
       <c r="B116" s="2">
         <v>1</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>817</v>
+      <c r="C116" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>722</v>
@@ -8904,8 +8943,8 @@
       <c r="B117" s="2">
         <v>2</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>817</v>
+      <c r="C117" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>723</v>
@@ -8918,8 +8957,8 @@
       <c r="B118" s="2">
         <v>0</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>817</v>
+      <c r="C118" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>704</v>
@@ -8932,8 +8971,8 @@
       <c r="B119" s="2">
         <v>1</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>817</v>
+      <c r="C119" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>705</v>
@@ -8946,8 +8985,8 @@
       <c r="B120" s="2">
         <v>0</v>
       </c>
-      <c r="C120" s="2" t="s">
-        <v>817</v>
+      <c r="C120" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>704</v>
@@ -8960,8 +8999,8 @@
       <c r="B121" s="2">
         <v>1</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>817</v>
+      <c r="C121" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>705</v>
@@ -8974,8 +9013,8 @@
       <c r="B122" s="2">
         <v>1</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>817</v>
+      <c r="C122" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>724</v>
@@ -8988,8 +9027,8 @@
       <c r="B123" s="2">
         <v>2</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>817</v>
+      <c r="C123" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>725</v>
@@ -9002,8 +9041,8 @@
       <c r="B124" s="2">
         <v>3</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>817</v>
+      <c r="C124" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>726</v>
@@ -9016,8 +9055,8 @@
       <c r="B125" s="2">
         <v>4</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>817</v>
+      <c r="C125" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>727</v>
@@ -9030,8 +9069,8 @@
       <c r="B126" s="2">
         <v>5</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>817</v>
+      <c r="C126" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>728</v>
@@ -9044,8 +9083,8 @@
       <c r="B127" s="2">
         <v>6</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>817</v>
+      <c r="C127" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>729</v>
@@ -9058,8 +9097,8 @@
       <c r="B128" s="2">
         <v>1</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>817</v>
+      <c r="C128" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>730</v>
@@ -9072,8 +9111,8 @@
       <c r="B129" s="2">
         <v>2</v>
       </c>
-      <c r="C129" s="2" t="s">
-        <v>817</v>
+      <c r="C129" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>731</v>
@@ -9086,8 +9125,8 @@
       <c r="B130" s="2">
         <v>3</v>
       </c>
-      <c r="C130" s="2" t="s">
-        <v>817</v>
+      <c r="C130" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>732</v>
@@ -9100,8 +9139,8 @@
       <c r="B131" s="2">
         <v>4</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>817</v>
+      <c r="C131" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>733</v>
@@ -9114,8 +9153,8 @@
       <c r="B132" s="2">
         <v>5</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>817</v>
+      <c r="C132" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>734</v>
@@ -9128,8 +9167,8 @@
       <c r="B133" s="2">
         <v>0</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>817</v>
+      <c r="C133" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>704</v>
@@ -9142,8 +9181,8 @@
       <c r="B134" s="2">
         <v>1</v>
       </c>
-      <c r="C134" s="2" t="s">
-        <v>817</v>
+      <c r="C134" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>705</v>
@@ -9156,8 +9195,8 @@
       <c r="B135" s="2">
         <v>0</v>
       </c>
-      <c r="C135" s="2" t="s">
-        <v>817</v>
+      <c r="C135" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>687</v>
@@ -9170,8 +9209,8 @@
       <c r="B136" s="2">
         <v>1</v>
       </c>
-      <c r="C136" s="2" t="s">
-        <v>817</v>
+      <c r="C136" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>688</v>
@@ -9184,8 +9223,8 @@
       <c r="B137" s="2">
         <v>2</v>
       </c>
-      <c r="C137" s="2" t="s">
-        <v>817</v>
+      <c r="C137" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>689</v>
@@ -9198,8 +9237,8 @@
       <c r="B138" s="2">
         <v>1</v>
       </c>
-      <c r="C138" s="2" t="s">
-        <v>817</v>
+      <c r="C138" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>735</v>
@@ -9212,8 +9251,8 @@
       <c r="B139" s="2">
         <v>2</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>817</v>
+      <c r="C139" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>736</v>
@@ -9226,8 +9265,8 @@
       <c r="B140" s="2">
         <v>3</v>
       </c>
-      <c r="C140" s="2" t="s">
-        <v>817</v>
+      <c r="C140" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>737</v>
@@ -9240,8 +9279,8 @@
       <c r="B141" s="2">
         <v>4</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>817</v>
+      <c r="C141" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>738</v>
@@ -9254,8 +9293,8 @@
       <c r="B142" s="2">
         <v>1</v>
       </c>
-      <c r="C142" s="2" t="s">
-        <v>817</v>
+      <c r="C142" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>739</v>
@@ -9268,8 +9307,8 @@
       <c r="B143" s="2">
         <v>2</v>
       </c>
-      <c r="C143" s="2" t="s">
-        <v>817</v>
+      <c r="C143" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>740</v>
@@ -9282,8 +9321,8 @@
       <c r="B144" s="2">
         <v>3</v>
       </c>
-      <c r="C144" s="2" t="s">
-        <v>817</v>
+      <c r="C144" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>741</v>
@@ -9296,8 +9335,8 @@
       <c r="B145" s="2">
         <v>1</v>
       </c>
-      <c r="C145" s="2" t="s">
-        <v>817</v>
+      <c r="C145" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>742</v>
@@ -9310,8 +9349,8 @@
       <c r="B146" s="2">
         <v>2</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>817</v>
+      <c r="C146" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>743</v>
@@ -9324,8 +9363,8 @@
       <c r="B147" s="2">
         <v>3</v>
       </c>
-      <c r="C147" s="2" t="s">
-        <v>817</v>
+      <c r="C147" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>741</v>
@@ -9338,8 +9377,8 @@
       <c r="B148" s="2">
         <v>1</v>
       </c>
-      <c r="C148" s="2" t="s">
-        <v>817</v>
+      <c r="C148" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>739</v>
@@ -9352,8 +9391,8 @@
       <c r="B149" s="2">
         <v>2</v>
       </c>
-      <c r="C149" s="2" t="s">
-        <v>817</v>
+      <c r="C149" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>740</v>
@@ -9366,8 +9405,8 @@
       <c r="B150" s="2">
         <v>3</v>
       </c>
-      <c r="C150" s="2" t="s">
-        <v>817</v>
+      <c r="C150" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>741</v>
@@ -9380,8 +9419,8 @@
       <c r="B151" s="2">
         <v>1</v>
       </c>
-      <c r="C151" s="2" t="s">
-        <v>817</v>
+      <c r="C151" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>735</v>
@@ -9394,8 +9433,8 @@
       <c r="B152" s="2">
         <v>2</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>817</v>
+      <c r="C152" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>736</v>
@@ -9408,8 +9447,8 @@
       <c r="B153" s="2">
         <v>3</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>817</v>
+      <c r="C153" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>737</v>
@@ -9422,8 +9461,8 @@
       <c r="B154" s="2">
         <v>4</v>
       </c>
-      <c r="C154" s="2" t="s">
-        <v>817</v>
+      <c r="C154" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>738</v>
@@ -9436,8 +9475,8 @@
       <c r="B155" s="2">
         <v>0</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>817</v>
+      <c r="C155" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>704</v>
@@ -9450,8 +9489,8 @@
       <c r="B156" s="2">
         <v>1</v>
       </c>
-      <c r="C156" s="2" t="s">
-        <v>817</v>
+      <c r="C156" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>705</v>
@@ -9464,8 +9503,8 @@
       <c r="B157" s="2">
         <v>1</v>
       </c>
-      <c r="C157" s="2" t="s">
-        <v>817</v>
+      <c r="C157" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>735</v>
@@ -9478,8 +9517,8 @@
       <c r="B158" s="2">
         <v>2</v>
       </c>
-      <c r="C158" s="2" t="s">
-        <v>817</v>
+      <c r="C158" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>736</v>
@@ -9492,8 +9531,8 @@
       <c r="B159" s="2">
         <v>3</v>
       </c>
-      <c r="C159" s="2" t="s">
-        <v>817</v>
+      <c r="C159" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>737</v>
@@ -9506,8 +9545,8 @@
       <c r="B160" s="2">
         <v>4</v>
       </c>
-      <c r="C160" s="2" t="s">
-        <v>817</v>
+      <c r="C160" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>738</v>
@@ -9520,8 +9559,8 @@
       <c r="B161" s="2">
         <v>0</v>
       </c>
-      <c r="C161" s="2" t="s">
-        <v>817</v>
+      <c r="C161" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>744</v>
@@ -9534,8 +9573,8 @@
       <c r="B162" s="2">
         <v>1</v>
       </c>
-      <c r="C162" s="2" t="s">
-        <v>817</v>
+      <c r="C162" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>745</v>
@@ -9548,8 +9587,8 @@
       <c r="B163" s="2">
         <v>2</v>
       </c>
-      <c r="C163" s="2" t="s">
-        <v>817</v>
+      <c r="C163" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D163" s="2" t="s">
         <v>746</v>
@@ -9562,8 +9601,8 @@
       <c r="B164" s="2">
         <v>1</v>
       </c>
-      <c r="C164" s="2" t="s">
-        <v>817</v>
+      <c r="C164" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D164" s="2" t="s">
         <v>735</v>
@@ -9576,8 +9615,8 @@
       <c r="B165" s="2">
         <v>2</v>
       </c>
-      <c r="C165" s="2" t="s">
-        <v>817</v>
+      <c r="C165" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D165" s="2" t="s">
         <v>736</v>
@@ -9590,8 +9629,8 @@
       <c r="B166" s="2">
         <v>3</v>
       </c>
-      <c r="C166" s="2" t="s">
-        <v>817</v>
+      <c r="C166" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>737</v>
@@ -9604,8 +9643,8 @@
       <c r="B167" s="2">
         <v>4</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>817</v>
+      <c r="C167" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>738</v>
@@ -9618,8 +9657,8 @@
       <c r="B168" s="2">
         <v>0</v>
       </c>
-      <c r="C168" s="2" t="s">
-        <v>817</v>
+      <c r="C168" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>744</v>
@@ -9632,8 +9671,8 @@
       <c r="B169" s="2">
         <v>1</v>
       </c>
-      <c r="C169" s="2" t="s">
-        <v>817</v>
+      <c r="C169" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D169" s="2" t="s">
         <v>745</v>
@@ -9646,8 +9685,8 @@
       <c r="B170" s="2">
         <v>2</v>
       </c>
-      <c r="C170" s="2" t="s">
-        <v>817</v>
+      <c r="C170" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>746</v>
@@ -9660,8 +9699,8 @@
       <c r="B171" s="2">
         <v>1</v>
       </c>
-      <c r="C171" s="2" t="s">
-        <v>817</v>
+      <c r="C171" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>735</v>
@@ -9674,8 +9713,8 @@
       <c r="B172" s="2">
         <v>2</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>817</v>
+      <c r="C172" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>736</v>
@@ -9688,8 +9727,8 @@
       <c r="B173" s="2">
         <v>3</v>
       </c>
-      <c r="C173" s="2" t="s">
-        <v>817</v>
+      <c r="C173" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>737</v>
@@ -9702,8 +9741,8 @@
       <c r="B174" s="2">
         <v>4</v>
       </c>
-      <c r="C174" s="2" t="s">
-        <v>817</v>
+      <c r="C174" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>738</v>
@@ -9716,8 +9755,8 @@
       <c r="B175" s="2">
         <v>1</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>817</v>
+      <c r="C175" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>695</v>
@@ -9730,8 +9769,8 @@
       <c r="B176" s="2">
         <v>2</v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>817</v>
+      <c r="C176" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>747</v>
@@ -9744,8 +9783,8 @@
       <c r="B177" s="2">
         <v>3</v>
       </c>
-      <c r="C177" s="2" t="s">
-        <v>817</v>
+      <c r="C177" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>748</v>
@@ -9758,8 +9797,8 @@
       <c r="B178" s="2">
         <v>4</v>
       </c>
-      <c r="C178" s="2" t="s">
-        <v>817</v>
+      <c r="C178" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>703</v>
@@ -9772,8 +9811,8 @@
       <c r="B179" s="2">
         <v>0</v>
       </c>
-      <c r="C179" s="2" t="s">
-        <v>817</v>
+      <c r="C179" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>704</v>
@@ -9786,8 +9825,8 @@
       <c r="B180" s="2">
         <v>1</v>
       </c>
-      <c r="C180" s="2" t="s">
-        <v>817</v>
+      <c r="C180" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>705</v>
@@ -9800,8 +9839,8 @@
       <c r="B181" s="2">
         <v>0</v>
       </c>
-      <c r="C181" s="2" t="s">
-        <v>817</v>
+      <c r="C181" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>704</v>
@@ -9814,8 +9853,8 @@
       <c r="B182" s="2">
         <v>1</v>
       </c>
-      <c r="C182" s="2" t="s">
-        <v>817</v>
+      <c r="C182" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>705</v>
@@ -9828,8 +9867,8 @@
       <c r="B183" s="2">
         <v>0</v>
       </c>
-      <c r="C183" s="2" t="s">
-        <v>817</v>
+      <c r="C183" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>704</v>
@@ -9842,8 +9881,8 @@
       <c r="B184" s="2">
         <v>1</v>
       </c>
-      <c r="C184" s="2" t="s">
-        <v>817</v>
+      <c r="C184" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>705</v>
@@ -9856,8 +9895,8 @@
       <c r="B185" s="2">
         <v>0</v>
       </c>
-      <c r="C185" s="2" t="s">
-        <v>817</v>
+      <c r="C185" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>749</v>
@@ -9870,8 +9909,8 @@
       <c r="B186" s="2">
         <v>1</v>
       </c>
-      <c r="C186" s="2" t="s">
-        <v>817</v>
+      <c r="C186" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>750</v>
@@ -9884,8 +9923,8 @@
       <c r="B187" s="2">
         <v>2</v>
       </c>
-      <c r="C187" s="2" t="s">
-        <v>817</v>
+      <c r="C187" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>751</v>
@@ -9898,8 +9937,8 @@
       <c r="B188" s="2">
         <v>1</v>
       </c>
-      <c r="C188" s="2" t="s">
-        <v>817</v>
+      <c r="C188" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>735</v>
@@ -9912,8 +9951,8 @@
       <c r="B189" s="2">
         <v>2</v>
       </c>
-      <c r="C189" s="2" t="s">
-        <v>817</v>
+      <c r="C189" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>736</v>
@@ -9926,8 +9965,8 @@
       <c r="B190" s="2">
         <v>3</v>
       </c>
-      <c r="C190" s="2" t="s">
-        <v>817</v>
+      <c r="C190" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>737</v>
@@ -9940,8 +9979,8 @@
       <c r="B191" s="2">
         <v>4</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>817</v>
+      <c r="C191" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>738</v>
@@ -9954,8 +9993,8 @@
       <c r="B192" s="2">
         <v>0</v>
       </c>
-      <c r="C192" s="2" t="s">
-        <v>817</v>
+      <c r="C192" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>704</v>
@@ -9968,8 +10007,8 @@
       <c r="B193" s="2">
         <v>1</v>
       </c>
-      <c r="C193" s="2" t="s">
-        <v>817</v>
+      <c r="C193" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>705</v>
@@ -9982,8 +10021,8 @@
       <c r="B194" s="2">
         <v>1</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>817</v>
+      <c r="C194" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>752</v>
@@ -9996,8 +10035,8 @@
       <c r="B195" s="2">
         <v>2</v>
       </c>
-      <c r="C195" s="2" t="s">
-        <v>817</v>
+      <c r="C195" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>753</v>
@@ -10010,8 +10049,8 @@
       <c r="B196" s="2">
         <v>1</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>817</v>
+      <c r="C196" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>754</v>
@@ -10024,8 +10063,8 @@
       <c r="B197" s="2">
         <v>2</v>
       </c>
-      <c r="C197" s="2" t="s">
-        <v>817</v>
+      <c r="C197" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>755</v>
@@ -10038,8 +10077,8 @@
       <c r="B198" s="2">
         <v>3</v>
       </c>
-      <c r="C198" s="2" t="s">
-        <v>817</v>
+      <c r="C198" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>756</v>
@@ -10052,8 +10091,8 @@
       <c r="B199" s="2">
         <v>1</v>
       </c>
-      <c r="C199" s="2" t="s">
-        <v>817</v>
+      <c r="C199" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>757</v>
@@ -10066,8 +10105,8 @@
       <c r="B200" s="2">
         <v>2</v>
       </c>
-      <c r="C200" s="2" t="s">
-        <v>817</v>
+      <c r="C200" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>758</v>
@@ -10080,8 +10119,8 @@
       <c r="B201" s="2">
         <v>3</v>
       </c>
-      <c r="C201" s="2" t="s">
-        <v>817</v>
+      <c r="C201" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>759</v>
@@ -10094,8 +10133,8 @@
       <c r="B202" s="2">
         <v>0</v>
       </c>
-      <c r="C202" s="2" t="s">
-        <v>817</v>
+      <c r="C202" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>704</v>
@@ -10108,8 +10147,8 @@
       <c r="B203" s="2">
         <v>1</v>
       </c>
-      <c r="C203" s="2" t="s">
-        <v>817</v>
+      <c r="C203" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>705</v>
@@ -10122,8 +10161,8 @@
       <c r="B204" s="2">
         <v>0</v>
       </c>
-      <c r="C204" s="2" t="s">
-        <v>817</v>
+      <c r="C204" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>704</v>
@@ -10136,8 +10175,8 @@
       <c r="B205" s="2">
         <v>1</v>
       </c>
-      <c r="C205" s="2" t="s">
-        <v>817</v>
+      <c r="C205" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>705</v>
@@ -10150,8 +10189,8 @@
       <c r="B206" s="2">
         <v>0</v>
       </c>
-      <c r="C206" s="2" t="s">
-        <v>817</v>
+      <c r="C206" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>704</v>
@@ -10164,8 +10203,8 @@
       <c r="B207" s="2">
         <v>1</v>
       </c>
-      <c r="C207" s="2" t="s">
-        <v>817</v>
+      <c r="C207" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>705</v>
@@ -10178,8 +10217,8 @@
       <c r="B208" s="2">
         <v>1</v>
       </c>
-      <c r="C208" s="2" t="s">
-        <v>817</v>
+      <c r="C208" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>718</v>
@@ -10192,8 +10231,8 @@
       <c r="B209" s="2">
         <v>2</v>
       </c>
-      <c r="C209" s="2" t="s">
-        <v>817</v>
+      <c r="C209" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D209" s="2" t="s">
         <v>719</v>
@@ -10206,8 +10245,8 @@
       <c r="B210" s="2">
         <v>3</v>
       </c>
-      <c r="C210" s="2" t="s">
-        <v>817</v>
+      <c r="C210" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>720</v>
@@ -10220,8 +10259,8 @@
       <c r="B211" s="2">
         <v>4</v>
       </c>
-      <c r="C211" s="2" t="s">
-        <v>817</v>
+      <c r="C211" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>760</v>
@@ -10234,8 +10273,8 @@
       <c r="B212" s="2">
         <v>5</v>
       </c>
-      <c r="C212" s="2" t="s">
-        <v>817</v>
+      <c r="C212" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D212" s="2" t="s">
         <v>761</v>
@@ -10248,8 +10287,8 @@
       <c r="B213" s="2">
         <v>0</v>
       </c>
-      <c r="C213" s="2" t="s">
-        <v>817</v>
+      <c r="C213" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>704</v>
@@ -10262,8 +10301,8 @@
       <c r="B214" s="2">
         <v>1</v>
       </c>
-      <c r="C214" s="2" t="s">
-        <v>817</v>
+      <c r="C214" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>705</v>
@@ -10276,8 +10315,8 @@
       <c r="B215" s="2">
         <v>0</v>
       </c>
-      <c r="C215" s="2" t="s">
-        <v>817</v>
+      <c r="C215" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>762</v>
@@ -10290,8 +10329,8 @@
       <c r="B216" s="2">
         <v>1</v>
       </c>
-      <c r="C216" s="2" t="s">
-        <v>817</v>
+      <c r="C216" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>763</v>
@@ -10304,8 +10343,8 @@
       <c r="B217" s="2">
         <v>1</v>
       </c>
-      <c r="C217" s="2" t="s">
-        <v>817</v>
+      <c r="C217" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>764</v>
@@ -10318,8 +10357,8 @@
       <c r="B218" s="2">
         <v>2</v>
       </c>
-      <c r="C218" s="2" t="s">
-        <v>817</v>
+      <c r="C218" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>765</v>
@@ -10332,8 +10371,8 @@
       <c r="B219" s="2">
         <v>3</v>
       </c>
-      <c r="C219" s="2" t="s">
-        <v>817</v>
+      <c r="C219" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>766</v>
@@ -10346,8 +10385,8 @@
       <c r="B220" s="2">
         <v>4</v>
       </c>
-      <c r="C220" s="2" t="s">
-        <v>817</v>
+      <c r="C220" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>767</v>
@@ -10360,8 +10399,8 @@
       <c r="B221" s="2">
         <v>5</v>
       </c>
-      <c r="C221" s="2" t="s">
-        <v>817</v>
+      <c r="C221" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D221" s="2" t="s">
         <v>768</v>
@@ -10374,8 +10413,8 @@
       <c r="B222" s="2">
         <v>1</v>
       </c>
-      <c r="C222" s="2" t="s">
-        <v>817</v>
+      <c r="C222" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D222" s="2" t="s">
         <v>769</v>
@@ -10388,8 +10427,8 @@
       <c r="B223" s="2">
         <v>2</v>
       </c>
-      <c r="C223" s="2" t="s">
-        <v>817</v>
+      <c r="C223" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D223" s="2" t="s">
         <v>770</v>
@@ -10402,8 +10441,8 @@
       <c r="B224" s="2">
         <v>3</v>
       </c>
-      <c r="C224" s="2" t="s">
-        <v>817</v>
+      <c r="C224" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D224" s="2" t="s">
         <v>771</v>
@@ -10416,8 +10455,8 @@
       <c r="B225" s="2">
         <v>4</v>
       </c>
-      <c r="C225" s="2" t="s">
-        <v>817</v>
+      <c r="C225" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D225" s="2" t="s">
         <v>772</v>
@@ -10430,8 +10469,8 @@
       <c r="B226" s="2">
         <v>5</v>
       </c>
-      <c r="C226" s="2" t="s">
-        <v>817</v>
+      <c r="C226" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D226" s="2" t="s">
         <v>773</v>
@@ -10444,8 +10483,8 @@
       <c r="B227" s="2">
         <v>0</v>
       </c>
-      <c r="C227" s="2" t="s">
-        <v>817</v>
+      <c r="C227" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D227" s="2" t="s">
         <v>774</v>
@@ -10458,8 +10497,8 @@
       <c r="B228" s="2">
         <v>1</v>
       </c>
-      <c r="C228" s="2" t="s">
-        <v>817</v>
+      <c r="C228" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D228" s="2" t="s">
         <v>775</v>
@@ -10472,8 +10511,8 @@
       <c r="B229" s="2">
         <v>2</v>
       </c>
-      <c r="C229" s="2" t="s">
-        <v>817</v>
+      <c r="C229" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D229" s="2" t="s">
         <v>776</v>
@@ -10486,8 +10525,8 @@
       <c r="B230" s="2">
         <v>3</v>
       </c>
-      <c r="C230" s="2" t="s">
-        <v>817</v>
+      <c r="C230" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D230" s="2" t="s">
         <v>777</v>
@@ -10500,8 +10539,8 @@
       <c r="B231" s="2">
         <v>4</v>
       </c>
-      <c r="C231" s="2" t="s">
-        <v>817</v>
+      <c r="C231" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D231" s="2" t="s">
         <v>778</v>
@@ -10514,8 +10553,8 @@
       <c r="B232" s="2">
         <v>5</v>
       </c>
-      <c r="C232" s="2" t="s">
-        <v>817</v>
+      <c r="C232" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D232" s="2" t="s">
         <v>779</v>
@@ -10528,8 +10567,8 @@
       <c r="B233" s="2">
         <v>6</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>817</v>
+      <c r="C233" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D233" s="2" t="s">
         <v>780</v>
@@ -10542,8 +10581,8 @@
       <c r="B234" s="2">
         <v>7</v>
       </c>
-      <c r="C234" s="2" t="s">
-        <v>817</v>
+      <c r="C234" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D234" s="2" t="s">
         <v>781</v>
@@ -10556,8 +10595,8 @@
       <c r="B235" s="2">
         <v>8</v>
       </c>
-      <c r="C235" s="2" t="s">
-        <v>817</v>
+      <c r="C235" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D235" s="2" t="s">
         <v>782</v>
@@ -10570,8 +10609,8 @@
       <c r="B236" s="2">
         <v>9</v>
       </c>
-      <c r="C236" s="2" t="s">
-        <v>817</v>
+      <c r="C236" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D236" s="2" t="s">
         <v>783</v>
@@ -10584,8 +10623,8 @@
       <c r="B237" s="2">
         <v>0</v>
       </c>
-      <c r="C237" s="2" t="s">
-        <v>817</v>
+      <c r="C237" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D237" s="2" t="s">
         <v>774</v>
@@ -10598,8 +10637,8 @@
       <c r="B238" s="2">
         <v>1</v>
       </c>
-      <c r="C238" s="2" t="s">
-        <v>817</v>
+      <c r="C238" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>775</v>
@@ -10612,8 +10651,8 @@
       <c r="B239" s="2">
         <v>2</v>
       </c>
-      <c r="C239" s="2" t="s">
-        <v>817</v>
+      <c r="C239" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D239" s="2" t="s">
         <v>776</v>
@@ -10626,8 +10665,8 @@
       <c r="B240" s="2">
         <v>3</v>
       </c>
-      <c r="C240" s="2" t="s">
-        <v>817</v>
+      <c r="C240" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>777</v>
@@ -10640,8 +10679,8 @@
       <c r="B241" s="2">
         <v>4</v>
       </c>
-      <c r="C241" s="2" t="s">
-        <v>817</v>
+      <c r="C241" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>778</v>
@@ -10654,8 +10693,8 @@
       <c r="B242" s="2">
         <v>5</v>
       </c>
-      <c r="C242" s="2" t="s">
-        <v>817</v>
+      <c r="C242" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>779</v>
@@ -10668,8 +10707,8 @@
       <c r="B243" s="2">
         <v>6</v>
       </c>
-      <c r="C243" s="2" t="s">
-        <v>817</v>
+      <c r="C243" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>780</v>
@@ -10682,8 +10721,8 @@
       <c r="B244" s="2">
         <v>7</v>
       </c>
-      <c r="C244" s="2" t="s">
-        <v>817</v>
+      <c r="C244" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>781</v>
@@ -10696,8 +10735,8 @@
       <c r="B245" s="2">
         <v>8</v>
       </c>
-      <c r="C245" s="2" t="s">
-        <v>817</v>
+      <c r="C245" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>782</v>
@@ -10710,8 +10749,8 @@
       <c r="B246" s="2">
         <v>9</v>
       </c>
-      <c r="C246" s="2" t="s">
-        <v>817</v>
+      <c r="C246" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>783</v>
@@ -10724,8 +10763,8 @@
       <c r="B247" s="2">
         <v>1001</v>
       </c>
-      <c r="C247" s="2" t="s">
-        <v>817</v>
+      <c r="C247" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>784</v>
@@ -10738,8 +10777,8 @@
       <c r="B248" s="2">
         <v>1102</v>
       </c>
-      <c r="C248" s="2" t="s">
-        <v>817</v>
+      <c r="C248" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>785</v>
@@ -10752,8 +10791,8 @@
       <c r="B249" s="2">
         <v>1103</v>
       </c>
-      <c r="C249" s="2" t="s">
-        <v>817</v>
+      <c r="C249" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>786</v>
@@ -10766,8 +10805,8 @@
       <c r="B250" s="2">
         <v>1104</v>
       </c>
-      <c r="C250" s="2" t="s">
-        <v>817</v>
+      <c r="C250" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>787</v>
@@ -10780,8 +10819,8 @@
       <c r="B251" s="2">
         <v>1201</v>
       </c>
-      <c r="C251" s="2" t="s">
-        <v>817</v>
+      <c r="C251" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>788</v>
@@ -10794,8 +10833,8 @@
       <c r="B252" s="2">
         <v>1202</v>
       </c>
-      <c r="C252" s="2" t="s">
-        <v>817</v>
+      <c r="C252" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>789</v>
@@ -10808,8 +10847,8 @@
       <c r="B253" s="2">
         <v>1203</v>
       </c>
-      <c r="C253" s="2" t="s">
-        <v>817</v>
+      <c r="C253" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D253" s="2" t="s">
         <v>790</v>
@@ -10822,8 +10861,8 @@
       <c r="B254" s="2">
         <v>1301</v>
       </c>
-      <c r="C254" s="2" t="s">
-        <v>817</v>
+      <c r="C254" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D254" s="2" t="s">
         <v>791</v>
@@ -10836,8 +10875,8 @@
       <c r="B255" s="2">
         <v>1401</v>
       </c>
-      <c r="C255" s="2" t="s">
-        <v>817</v>
+      <c r="C255" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D255" s="2" t="s">
         <v>792</v>
@@ -10850,8 +10889,8 @@
       <c r="B256" s="2">
         <v>1501</v>
       </c>
-      <c r="C256" s="2" t="s">
-        <v>817</v>
+      <c r="C256" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D256" s="2" t="s">
         <v>793</v>
@@ -10864,8 +10903,8 @@
       <c r="B257" s="2">
         <v>1601</v>
       </c>
-      <c r="C257" s="2" t="s">
-        <v>817</v>
+      <c r="C257" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D257" s="2" t="s">
         <v>794</v>
@@ -10878,8 +10917,8 @@
       <c r="B258" s="2">
         <v>1701</v>
       </c>
-      <c r="C258" s="2" t="s">
-        <v>817</v>
+      <c r="C258" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D258" s="2" t="s">
         <v>795</v>
@@ -10892,8 +10931,8 @@
       <c r="B259" s="2">
         <v>1801</v>
       </c>
-      <c r="C259" s="2" t="s">
-        <v>817</v>
+      <c r="C259" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D259" s="2" t="s">
         <v>796</v>
@@ -10906,8 +10945,8 @@
       <c r="B260" s="2">
         <v>1802</v>
       </c>
-      <c r="C260" s="2" t="s">
-        <v>817</v>
+      <c r="C260" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>797</v>
@@ -10920,8 +10959,8 @@
       <c r="B261" s="2">
         <v>1901</v>
       </c>
-      <c r="C261" s="2" t="s">
-        <v>817</v>
+      <c r="C261" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>798</v>
@@ -10934,8 +10973,8 @@
       <c r="B262" s="2">
         <v>2001</v>
       </c>
-      <c r="C262" s="2" t="s">
-        <v>817</v>
+      <c r="C262" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>799</v>
@@ -10948,8 +10987,8 @@
       <c r="B263" s="2">
         <v>1</v>
       </c>
-      <c r="C263" s="2" t="s">
-        <v>817</v>
+      <c r="C263" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D263" s="2" t="s">
         <v>705</v>
@@ -10962,8 +11001,8 @@
       <c r="B264" s="2">
         <v>0</v>
       </c>
-      <c r="C264" s="2" t="s">
-        <v>817</v>
+      <c r="C264" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>704</v>
@@ -10976,8 +11015,8 @@
       <c r="B265" s="2">
         <v>1</v>
       </c>
-      <c r="C265" s="2" t="s">
-        <v>817</v>
+      <c r="C265" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D265" s="2" t="s">
         <v>705</v>
@@ -10990,8 +11029,8 @@
       <c r="B266" s="2">
         <v>0</v>
       </c>
-      <c r="C266" s="2" t="s">
-        <v>817</v>
+      <c r="C266" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D266" s="2" t="s">
         <v>704</v>
@@ -11004,8 +11043,8 @@
       <c r="B267" s="2">
         <v>1</v>
       </c>
-      <c r="C267" s="2" t="s">
-        <v>817</v>
+      <c r="C267" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D267" s="2" t="s">
         <v>800</v>
@@ -11018,8 +11057,8 @@
       <c r="B268" s="2">
         <v>2</v>
       </c>
-      <c r="C268" s="2" t="s">
-        <v>817</v>
+      <c r="C268" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D268" s="2" t="s">
         <v>801</v>
@@ -11032,8 +11071,8 @@
       <c r="B269" s="2">
         <v>3</v>
       </c>
-      <c r="C269" s="2" t="s">
-        <v>817</v>
+      <c r="C269" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D269" s="2" t="s">
         <v>802</v>
@@ -11046,8 +11085,8 @@
       <c r="B270" s="2">
         <v>4</v>
       </c>
-      <c r="C270" s="2" t="s">
-        <v>817</v>
+      <c r="C270" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>803</v>
@@ -11060,8 +11099,8 @@
       <c r="B271" s="2">
         <v>5</v>
       </c>
-      <c r="C271" s="2" t="s">
-        <v>817</v>
+      <c r="C271" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>804</v>
@@ -11074,8 +11113,8 @@
       <c r="B272" s="2">
         <v>6</v>
       </c>
-      <c r="C272" s="2" t="s">
-        <v>817</v>
+      <c r="C272" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D272" s="2" t="s">
         <v>805</v>
@@ -11088,8 +11127,8 @@
       <c r="B273" s="2">
         <v>1</v>
       </c>
-      <c r="C273" s="2" t="s">
-        <v>817</v>
+      <c r="C273" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D273" s="2" t="s">
         <v>806</v>
@@ -11102,8 +11141,8 @@
       <c r="B274" s="2">
         <v>2</v>
       </c>
-      <c r="C274" s="2" t="s">
-        <v>817</v>
+      <c r="C274" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D274" s="2" t="s">
         <v>802</v>
@@ -11116,8 +11155,8 @@
       <c r="B275" s="2">
         <v>3</v>
       </c>
-      <c r="C275" s="2" t="s">
-        <v>817</v>
+      <c r="C275" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>803</v>
@@ -11130,8 +11169,8 @@
       <c r="B276" s="2">
         <v>4</v>
       </c>
-      <c r="C276" s="2" t="s">
-        <v>817</v>
+      <c r="C276" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D276" s="2" t="s">
         <v>804</v>
@@ -11144,8 +11183,8 @@
       <c r="B277" s="2">
         <v>5</v>
       </c>
-      <c r="C277" s="2" t="s">
-        <v>817</v>
+      <c r="C277" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D277" s="2" t="s">
         <v>807</v>
@@ -11158,8 +11197,8 @@
       <c r="B278" s="2">
         <v>6</v>
       </c>
-      <c r="C278" s="2" t="s">
-        <v>817</v>
+      <c r="C278" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D278" s="2" t="s">
         <v>808</v>
@@ -11172,8 +11211,8 @@
       <c r="B279" s="2">
         <v>1</v>
       </c>
-      <c r="C279" s="2" t="s">
-        <v>817</v>
+      <c r="C279" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D279" s="2" t="s">
         <v>809</v>
@@ -11186,8 +11225,8 @@
       <c r="B280" s="2">
         <v>2</v>
       </c>
-      <c r="C280" s="2" t="s">
-        <v>817</v>
+      <c r="C280" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D280" s="2" t="s">
         <v>810</v>
@@ -11200,8 +11239,8 @@
       <c r="B281" s="2">
         <v>3</v>
       </c>
-      <c r="C281" s="2" t="s">
-        <v>817</v>
+      <c r="C281" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D281" s="2" t="s">
         <v>811</v>
@@ -11214,8 +11253,8 @@
       <c r="B282" s="2">
         <v>1</v>
       </c>
-      <c r="C282" s="2" t="s">
-        <v>817</v>
+      <c r="C282" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D282" s="2" t="s">
         <v>809</v>
@@ -11228,8 +11267,8 @@
       <c r="B283" s="2">
         <v>2</v>
       </c>
-      <c r="C283" s="2" t="s">
-        <v>817</v>
+      <c r="C283" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D283" s="2" t="s">
         <v>812</v>
@@ -11242,8 +11281,8 @@
       <c r="B284" s="2">
         <v>3</v>
       </c>
-      <c r="C284" s="2" t="s">
-        <v>817</v>
+      <c r="C284" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D284" s="2" t="s">
         <v>810</v>
@@ -11256,8 +11295,8 @@
       <c r="B285" s="2">
         <v>4</v>
       </c>
-      <c r="C285" s="2" t="s">
-        <v>817</v>
+      <c r="C285" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D285" s="2" t="s">
         <v>813</v>
@@ -11270,8 +11309,8 @@
       <c r="B286" s="2">
         <v>5</v>
       </c>
-      <c r="C286" s="2" t="s">
-        <v>817</v>
+      <c r="C286" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D286" s="2" t="s">
         <v>811</v>
@@ -11284,8 +11323,8 @@
       <c r="B287" s="2">
         <v>1</v>
       </c>
-      <c r="C287" s="2" t="s">
-        <v>817</v>
+      <c r="C287" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D287" s="2" t="s">
         <v>814</v>
@@ -11298,8 +11337,8 @@
       <c r="B288" s="2">
         <v>2</v>
       </c>
-      <c r="C288" s="2" t="s">
-        <v>817</v>
+      <c r="C288" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D288" s="2" t="s">
         <v>815</v>
@@ -11312,8 +11351,8 @@
       <c r="B289" s="2">
         <v>3</v>
       </c>
-      <c r="C289" s="2" t="s">
-        <v>817</v>
+      <c r="C289" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D289" s="2" t="s">
         <v>816</v>
@@ -11326,8 +11365,8 @@
       <c r="B290" s="2">
         <v>1</v>
       </c>
-      <c r="C290" s="2" t="s">
-        <v>817</v>
+      <c r="C290" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D290" s="2" t="s">
         <v>814</v>
@@ -11340,8 +11379,8 @@
       <c r="B291" s="2">
         <v>2</v>
       </c>
-      <c r="C291" s="2" t="s">
-        <v>817</v>
+      <c r="C291" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D291" s="2" t="s">
         <v>815</v>
@@ -11354,8 +11393,8 @@
       <c r="B292" s="2">
         <v>3</v>
       </c>
-      <c r="C292" s="2" t="s">
-        <v>817</v>
+      <c r="C292" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D292" s="2" t="s">
         <v>816</v>
@@ -11368,8 +11407,8 @@
       <c r="B293" s="2">
         <v>1</v>
       </c>
-      <c r="C293" s="2" t="s">
-        <v>817</v>
+      <c r="C293" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D293" s="2" t="s">
         <v>814</v>
@@ -11382,8 +11421,8 @@
       <c r="B294" s="2">
         <v>2</v>
       </c>
-      <c r="C294" s="2" t="s">
-        <v>817</v>
+      <c r="C294" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D294" s="2" t="s">
         <v>815</v>
@@ -11396,8 +11435,8 @@
       <c r="B295" s="2">
         <v>3</v>
       </c>
-      <c r="C295" s="2" t="s">
-        <v>817</v>
+      <c r="C295" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D295" s="2" t="s">
         <v>816</v>
@@ -11410,8 +11449,8 @@
       <c r="B296" s="2">
         <v>0</v>
       </c>
-      <c r="C296" s="2" t="s">
-        <v>817</v>
+      <c r="C296" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>695</v>
@@ -11424,8 +11463,8 @@
       <c r="B297" s="2">
         <v>1</v>
       </c>
-      <c r="C297" s="2" t="s">
-        <v>817</v>
+      <c r="C297" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>696</v>
@@ -11438,8 +11477,8 @@
       <c r="B298" s="2">
         <v>0</v>
       </c>
-      <c r="C298" s="2" t="s">
-        <v>817</v>
+      <c r="C298" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>695</v>
@@ -11452,8 +11491,8 @@
       <c r="B299" s="2">
         <v>1</v>
       </c>
-      <c r="C299" s="2" t="s">
-        <v>817</v>
+      <c r="C299" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>696</v>
@@ -11466,8 +11505,8 @@
       <c r="B300" s="2">
         <v>0</v>
       </c>
-      <c r="C300" s="2" t="s">
-        <v>817</v>
+      <c r="C300" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D300" s="2" t="s">
         <v>695</v>
@@ -11480,8 +11519,8 @@
       <c r="B301" s="2">
         <v>1</v>
       </c>
-      <c r="C301" s="2" t="s">
-        <v>817</v>
+      <c r="C301" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D301" s="2" t="s">
         <v>696</v>

</xml_diff>

<commit_message>
feat(meta-vars): changes types of child_id to text and added metavars
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_non_repeated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474B4FF0-F4F7-4746-836B-5022AC0F1699}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81B1A3D-6D77-B444-98D4-0265E667A597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="818">
   <si>
     <t>name</t>
   </si>
@@ -2472,6 +2472,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -2499,7 +2502,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2891,8 +2894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D313"/>
   <sheetViews>
-    <sheetView topLeftCell="A283" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -2937,11 +2940,9 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>317</v>
-      </c>
+        <v>817</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>355</v>
       </c>
@@ -2951,11 +2952,9 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>317</v>
-      </c>
+        <v>817</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>356</v>
       </c>
@@ -7298,9 +7297,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A259" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C301"/>
+      <selection pane="bottomLeft" activeCell="B263" sqref="B263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>